<commit_message>
KING aanpasingen xlsx en minors
</commit_message>
<xml_diff>
--- a/src/main/resources/input/KING/props/KING.xlsx
+++ b/src/main/resources/input/KING/props/KING.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="416">
   <si>
     <t>Name</t>
   </si>
@@ -1297,6 +1297,9 @@
   </si>
   <si>
     <t>BSM: uitgebreid</t>
+  </si>
+  <si>
+    <t>VNGRSIM</t>
   </si>
 </sst>
 </file>
@@ -1969,11 +1972,11 @@
   <dimension ref="A1:W151"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="C93" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E64" sqref="E64"/>
       <selection pane="topRight" activeCell="E64" sqref="E64"/>
       <selection pane="bottomLeft" activeCell="E64" sqref="E64"/>
-      <selection pane="bottomRight" activeCell="F32" sqref="F32"/>
+      <selection pane="bottomRight" activeCell="M106" sqref="M106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4360,16 +4363,16 @@
       </c>
       <c r="G72" s="15"/>
       <c r="H72" s="45" t="s">
-        <v>290</v>
+        <v>415</v>
       </c>
       <c r="I72" s="45" t="s">
-        <v>290</v>
+        <v>415</v>
       </c>
       <c r="J72" s="45" t="s">
-        <v>290</v>
+        <v>415</v>
       </c>
       <c r="K72" s="45" t="s">
-        <v>290</v>
+        <v>415</v>
       </c>
       <c r="L72" s="22"/>
       <c r="M72" s="45" t="s">
@@ -5496,17 +5499,17 @@
         <v>404</v>
       </c>
       <c r="G106" s="15"/>
-      <c r="H106" s="34" t="s">
-        <v>290</v>
-      </c>
-      <c r="I106" s="59" t="s">
-        <v>290</v>
-      </c>
-      <c r="J106" s="59" t="s">
-        <v>290</v>
-      </c>
-      <c r="K106" s="59" t="s">
-        <v>290</v>
+      <c r="H106" s="45" t="s">
+        <v>415</v>
+      </c>
+      <c r="I106" s="45" t="s">
+        <v>415</v>
+      </c>
+      <c r="J106" s="45" t="s">
+        <v>415</v>
+      </c>
+      <c r="K106" s="45" t="s">
+        <v>415</v>
       </c>
       <c r="L106" s="22"/>
       <c r="M106" s="38" t="s">
@@ -6437,16 +6440,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="V45:V46"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
     <mergeCell ref="V7:V8"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="V45:V46"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D45:D46"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Enabled Toolbox generation for CIM, UGM and BSM.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/KING/props/KING.xlsx
+++ b/src/main/resources/input/KING/props/KING.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\KING\props\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\KING\Kern-taken\Imvertor\Imvertor-Maven\src\main\resources\input\KING\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0A3C9C-463F-44F1-BAA1-A75676DB08E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5280" windowWidth="29040" windowHeight="16440"/>
+    <workbookView xWindow="-28920" yWindow="5280" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KING" sheetId="3" r:id="rId1"/>
     <sheet name="Explanation" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="419">
   <si>
     <t>Name</t>
   </si>
@@ -1314,7 +1315,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1703,27 +1704,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="4" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="4" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
-    <cellStyle name="Explanatory Text" xfId="3" builtinId="53"/>
-    <cellStyle name="Good" xfId="4" builtinId="26"/>
+    <cellStyle name="Controlecel" xfId="1" builtinId="23"/>
+    <cellStyle name="Goed" xfId="4" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
-    <cellStyle name="Neutral 2" xfId="6"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Neutral 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Ongeldig" xfId="2" builtinId="27"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Verklarende tekst" xfId="3" builtinId="53"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2000,46 +2001,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:W153"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="C106" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E64" sqref="E64"/>
       <selection pane="topRight" activeCell="E64" sqref="E64"/>
       <selection pane="bottomLeft" activeCell="E64" sqref="E64"/>
-      <selection pane="bottomRight" activeCell="H120" sqref="H120:U120"/>
+      <selection pane="bottomRight" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="23.84375" customWidth="1"/>
-    <col min="2" max="2" width="20.15234375" customWidth="1"/>
-    <col min="3" max="3" width="50.69140625" customWidth="1"/>
-    <col min="4" max="4" width="10.84375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.86328125" customWidth="1"/>
+    <col min="2" max="2" width="20.1328125" customWidth="1"/>
+    <col min="3" max="3" width="50.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.86328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="2.69140625" style="18" customWidth="1"/>
-    <col min="8" max="8" width="16.61328125" customWidth="1"/>
-    <col min="9" max="9" width="14.69140625" customWidth="1"/>
-    <col min="10" max="10" width="14.3046875" customWidth="1"/>
-    <col min="11" max="11" width="15.69140625" customWidth="1"/>
-    <col min="12" max="12" width="2.3828125" style="18" customWidth="1"/>
-    <col min="13" max="13" width="18.69140625" customWidth="1"/>
-    <col min="14" max="14" width="16.07421875" customWidth="1"/>
-    <col min="15" max="16" width="15.69140625" customWidth="1"/>
-    <col min="17" max="17" width="2.3828125" style="18" customWidth="1"/>
-    <col min="18" max="18" width="19.921875" customWidth="1"/>
-    <col min="19" max="19" width="19.61328125" customWidth="1"/>
+    <col min="7" max="7" width="2.6640625" style="18" customWidth="1"/>
+    <col min="8" max="8" width="16.59765625" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" customWidth="1"/>
+    <col min="12" max="12" width="2.3984375" style="18" customWidth="1"/>
+    <col min="13" max="13" width="18.6640625" customWidth="1"/>
+    <col min="14" max="14" width="16.06640625" customWidth="1"/>
+    <col min="15" max="16" width="15.6640625" customWidth="1"/>
+    <col min="17" max="17" width="2.3984375" style="18" customWidth="1"/>
+    <col min="18" max="18" width="19.9296875" customWidth="1"/>
+    <col min="19" max="19" width="19.59765625" customWidth="1"/>
     <col min="20" max="21" width="18" customWidth="1"/>
-    <col min="22" max="22" width="63.61328125" customWidth="1"/>
-    <col min="23" max="23" width="30.07421875" customWidth="1"/>
+    <col min="22" max="22" width="63.59765625" customWidth="1"/>
+    <col min="23" max="23" width="30.06640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="3" customFormat="1" ht="37.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:23" s="3" customFormat="1" ht="36.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2101,7 +2102,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="3" customFormat="1" ht="56.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:23" s="3" customFormat="1" ht="56.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="F2" s="57"/>
       <c r="G2" s="14"/>
       <c r="H2" s="2" t="s">
@@ -2143,7 +2144,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="3" spans="1:23" s="1" customFormat="1" ht="29.6" thickTop="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:23" s="1" customFormat="1" ht="28.9" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>153</v>
       </c>
@@ -2172,7 +2173,7 @@
       <c r="T3" s="31"/>
       <c r="U3" s="31"/>
     </row>
-    <row r="4" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:23" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -2203,7 +2204,7 @@
       <c r="T4" s="31"/>
       <c r="U4" s="31"/>
     </row>
-    <row r="5" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -2234,7 +2235,7 @@
       <c r="T5" s="31"/>
       <c r="U5" s="31"/>
     </row>
-    <row r="6" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>156</v>
       </c>
@@ -2255,17 +2256,17 @@
       <c r="L6" s="15"/>
       <c r="Q6" s="22"/>
     </row>
-    <row r="7" spans="1:23" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A7" s="73" t="s">
+    <row r="7" spans="1:23" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A7" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="73" t="s">
+      <c r="C7" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="73" t="b">
+      <c r="D7" s="75" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="b">
@@ -2283,18 +2284,18 @@
       <c r="S7" s="31"/>
       <c r="T7" s="31"/>
       <c r="U7" s="31"/>
-      <c r="V7" s="72" t="s">
+      <c r="V7" s="74" t="s">
         <v>351</v>
       </c>
       <c r="W7" s="1" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="8" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="73"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
+    <row r="8" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="75"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="75"/>
       <c r="F8" s="51"/>
       <c r="G8" s="15"/>
       <c r="L8" s="15"/>
@@ -2307,9 +2308,9 @@
       <c r="S8" s="31"/>
       <c r="T8" s="31"/>
       <c r="U8" s="31"/>
-      <c r="V8" s="72"/>
-    </row>
-    <row r="9" spans="1:23" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="V8" s="74"/>
+    </row>
+    <row r="9" spans="1:23" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
         <v>159</v>
       </c>
@@ -2338,7 +2339,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="10" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:23" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -2369,7 +2370,7 @@
       <c r="T10" s="31"/>
       <c r="U10" s="31"/>
     </row>
-    <row r="11" spans="1:23" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:23" s="4" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
         <v>161</v>
       </c>
@@ -2390,7 +2391,7 @@
       <c r="L11" s="15"/>
       <c r="Q11" s="22"/>
     </row>
-    <row r="12" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:23" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
         <v>134</v>
       </c>
@@ -2419,7 +2420,7 @@
       <c r="T12" s="31"/>
       <c r="U12" s="31"/>
     </row>
-    <row r="13" spans="1:23" s="8" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:23" s="8" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
         <v>237</v>
       </c>
@@ -2454,7 +2455,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="14" spans="1:23" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:23" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -2485,7 +2486,7 @@
       <c r="T14" s="31"/>
       <c r="U14" s="31"/>
     </row>
-    <row r="15" spans="1:23" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:23" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -2522,7 +2523,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="16" spans="1:23" s="1" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:23" s="1" customFormat="1" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -2557,7 +2558,7 @@
       </c>
       <c r="W16" s="59"/>
     </row>
-    <row r="17" spans="1:23" s="1" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:23" s="1" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>215</v>
       </c>
@@ -2588,7 +2589,7 @@
       <c r="T17" s="31"/>
       <c r="U17" s="31"/>
     </row>
-    <row r="18" spans="1:23" s="1" customFormat="1" ht="156.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:23" s="1" customFormat="1" ht="156.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>217</v>
       </c>
@@ -2653,7 +2654,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="19" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:23" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>163</v>
       </c>
@@ -2684,7 +2685,7 @@
       <c r="T19" s="31"/>
       <c r="U19" s="31"/>
     </row>
-    <row r="20" spans="1:23" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:23" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>136</v>
       </c>
@@ -2721,7 +2722,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="21" spans="1:23" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:23" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>139</v>
       </c>
@@ -2759,7 +2760,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="22" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:23" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>142</v>
       </c>
@@ -2796,7 +2797,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="23" spans="1:23" s="4" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:23" s="4" customFormat="1" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A23" s="32" t="s">
         <v>25</v>
       </c>
@@ -2828,7 +2829,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="24" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A24" s="4" t="s">
         <v>165</v>
       </c>
@@ -2857,7 +2858,7 @@
       <c r="T24" s="31"/>
       <c r="U24" s="31"/>
     </row>
-    <row r="25" spans="1:23" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:23" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
@@ -2894,7 +2895,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="26" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:23" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
@@ -2914,21 +2915,28 @@
         <v>16</v>
       </c>
       <c r="G26" s="15"/>
+      <c r="I26" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="L26" s="15"/>
       <c r="M26" s="38"/>
-      <c r="N26" s="38"/>
+      <c r="N26" s="38" t="s">
+        <v>4</v>
+      </c>
       <c r="O26" s="38"/>
       <c r="P26" s="38"/>
       <c r="Q26" s="22"/>
       <c r="R26" s="31"/>
-      <c r="S26" s="59"/>
+      <c r="S26" s="59" t="s">
+        <v>4</v>
+      </c>
       <c r="T26" s="59"/>
       <c r="U26" s="59"/>
       <c r="V26" s="43" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="27" spans="1:23" s="70" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:23" s="70" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A27" s="70" t="s">
         <v>416</v>
       </c>
@@ -2948,13 +2956,22 @@
         <v>4</v>
       </c>
       <c r="G27" s="22"/>
+      <c r="I27" s="70" t="s">
+        <v>4</v>
+      </c>
       <c r="L27" s="22"/>
+      <c r="N27" s="70" t="s">
+        <v>4</v>
+      </c>
       <c r="Q27" s="22"/>
+      <c r="S27" s="70" t="s">
+        <v>4</v>
+      </c>
       <c r="V27" s="58" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="28" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:23" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
@@ -2988,7 +3005,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="29" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:23" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>144</v>
       </c>
@@ -3022,7 +3039,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="30" spans="1:23" s="37" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:23" s="37" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A30" s="4" t="s">
         <v>288</v>
       </c>
@@ -3047,7 +3064,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="31" spans="1:23" s="23" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:23" s="23" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A31" s="4" t="s">
         <v>250</v>
       </c>
@@ -3082,7 +3099,7 @@
       </c>
       <c r="W31" s="50"/>
     </row>
-    <row r="32" spans="1:23" s="25" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:23" s="25" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A32" s="4" t="s">
         <v>255</v>
       </c>
@@ -3121,7 +3138,7 @@
       </c>
       <c r="W32" s="50"/>
     </row>
-    <row r="33" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:23" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
@@ -3161,7 +3178,7 @@
       <c r="T33" s="59"/>
       <c r="U33" s="59"/>
     </row>
-    <row r="34" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:23" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>167</v>
       </c>
@@ -3192,7 +3209,7 @@
       <c r="T34" s="31"/>
       <c r="U34" s="31"/>
     </row>
-    <row r="35" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>170</v>
       </c>
@@ -3224,7 +3241,7 @@
       <c r="U35" s="31"/>
       <c r="V35" s="43"/>
     </row>
-    <row r="36" spans="1:23" s="30" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:23" s="30" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A36" s="30" t="s">
         <v>260</v>
       </c>
@@ -3253,7 +3270,7 @@
       <c r="U36" s="31"/>
       <c r="V36" s="43"/>
     </row>
-    <row r="37" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A37" s="4" t="s">
         <v>37</v>
       </c>
@@ -3283,7 +3300,7 @@
       <c r="T37" s="31"/>
       <c r="U37" s="31"/>
     </row>
-    <row r="38" spans="1:23" s="32" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:23" s="32" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A38" s="4" t="s">
         <v>272</v>
       </c>
@@ -3309,7 +3326,7 @@
       </c>
       <c r="W38" s="50"/>
     </row>
-    <row r="39" spans="1:23" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:23" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
@@ -3341,7 +3358,7 @@
       <c r="T39" s="31"/>
       <c r="U39" s="31"/>
     </row>
-    <row r="40" spans="1:23" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:23" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>41</v>
       </c>
@@ -3379,7 +3396,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="41" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>43</v>
       </c>
@@ -3411,7 +3428,7 @@
       <c r="T41" s="31"/>
       <c r="U41" s="31"/>
     </row>
-    <row r="42" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A42" s="4" t="s">
         <v>254</v>
       </c>
@@ -3446,7 +3463,7 @@
       <c r="T42" s="59"/>
       <c r="U42" s="59"/>
     </row>
-    <row r="43" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:23" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>173</v>
       </c>
@@ -3486,7 +3503,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="44" spans="1:23" s="4" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:23" s="4" customFormat="1" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A44" s="32" t="s">
         <v>45</v>
       </c>
@@ -3521,7 +3538,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="45" spans="1:23" s="4" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:23" s="4" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="44" t="s">
         <v>47</v>
       </c>
@@ -3553,17 +3570,17 @@
         <v>393</v>
       </c>
     </row>
-    <row r="46" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="73" t="s">
+    <row r="46" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A46" s="75" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="73" t="s">
+      <c r="B46" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="C46" s="73" t="s">
+      <c r="C46" s="75" t="s">
         <v>51</v>
       </c>
-      <c r="D46" s="73" t="b">
+      <c r="D46" s="75" t="b">
         <v>0</v>
       </c>
       <c r="E46" s="1" t="b">
@@ -3583,18 +3600,18 @@
       <c r="S46" s="45"/>
       <c r="T46" s="31"/>
       <c r="U46" s="31"/>
-      <c r="V46" s="72" t="s">
+      <c r="V46" s="74" t="s">
         <v>351</v>
       </c>
       <c r="W46" s="1" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="47" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="73"/>
-      <c r="B47" s="73"/>
-      <c r="C47" s="73"/>
-      <c r="D47" s="73"/>
+    <row r="47" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A47" s="75"/>
+      <c r="B47" s="75"/>
+      <c r="C47" s="75"/>
+      <c r="D47" s="75"/>
       <c r="F47" s="51"/>
       <c r="G47" s="15"/>
       <c r="L47" s="15"/>
@@ -3607,9 +3624,9 @@
       <c r="S47" s="31"/>
       <c r="T47" s="31"/>
       <c r="U47" s="31"/>
-      <c r="V47" s="72"/>
-    </row>
-    <row r="48" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="V47" s="74"/>
+    </row>
+    <row r="48" spans="1:23" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>175</v>
       </c>
@@ -3638,7 +3655,7 @@
       <c r="T48" s="31"/>
       <c r="U48" s="31"/>
     </row>
-    <row r="49" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>52</v>
       </c>
@@ -3669,7 +3686,7 @@
       <c r="T49" s="31"/>
       <c r="U49" s="31"/>
     </row>
-    <row r="50" spans="1:23" s="1" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:23" s="1" customFormat="1" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A50" s="4" t="s">
         <v>54</v>
       </c>
@@ -3706,7 +3723,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="51" spans="1:23" s="1" customFormat="1" ht="160.30000000000001" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:23" s="1" customFormat="1" ht="156.75" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
         <v>213</v>
       </c>
@@ -3769,7 +3786,7 @@
       </c>
       <c r="W51"/>
     </row>
-    <row r="52" spans="1:23" s="4" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:23" s="4" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="32" t="s">
         <v>178</v>
       </c>
@@ -3795,7 +3812,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="53" spans="1:23" s="4" customFormat="1" ht="86.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:23" s="4" customFormat="1" ht="86.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="32" t="s">
         <v>180</v>
       </c>
@@ -3831,7 +3848,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="54" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A54" s="4" t="s">
         <v>57</v>
       </c>
@@ -3861,7 +3878,7 @@
       <c r="U54" s="31"/>
       <c r="V54" s="43"/>
     </row>
-    <row r="55" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:23" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A55" s="4" t="s">
         <v>59</v>
       </c>
@@ -3896,7 +3913,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="56" spans="1:23" s="4" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:23" s="4" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="4" t="s">
         <v>61</v>
       </c>
@@ -3926,7 +3943,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="57" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:23" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A57" s="4" t="s">
         <v>183</v>
       </c>
@@ -3958,7 +3975,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="58" spans="1:23" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:23" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A58" s="65" t="s">
         <v>278</v>
       </c>
@@ -3992,7 +4009,7 @@
       </c>
       <c r="W58" s="50"/>
     </row>
-    <row r="59" spans="1:23" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:23" s="4" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A59" s="4" t="s">
         <v>280</v>
       </c>
@@ -4017,7 +4034,7 @@
       </c>
       <c r="W59" s="50"/>
     </row>
-    <row r="60" spans="1:23" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:23" s="4" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A60" s="4" t="s">
         <v>185</v>
       </c>
@@ -4040,7 +4057,7 @@
       <c r="V60" s="43"/>
       <c r="W60" s="50"/>
     </row>
-    <row r="61" spans="1:23" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:23" s="4" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A61" s="4" t="s">
         <v>283</v>
       </c>
@@ -4073,7 +4090,7 @@
       </c>
       <c r="W61" s="50"/>
     </row>
-    <row r="62" spans="1:23" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:23" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A62" s="11" t="s">
         <v>233</v>
       </c>
@@ -4112,7 +4129,7 @@
       </c>
       <c r="W62" s="50"/>
     </row>
-    <row r="63" spans="1:23" s="4" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:23" s="4" customFormat="1" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A63" s="4" t="s">
         <v>187</v>
       </c>
@@ -4138,7 +4155,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="64" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A64" s="4" t="s">
         <v>63</v>
       </c>
@@ -4171,7 +4188,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="65" spans="1:23" s="37" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:23" s="37" customFormat="1" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A65" s="4" t="s">
         <v>295</v>
       </c>
@@ -4199,7 +4216,7 @@
       </c>
       <c r="W65" s="61"/>
     </row>
-    <row r="66" spans="1:23" s="4" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:23" s="4" customFormat="1" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A66" s="4" t="s">
         <v>65</v>
       </c>
@@ -4225,7 +4242,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="67" spans="1:23" s="4" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:23" s="4" customFormat="1" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A67" s="4" t="s">
         <v>297</v>
       </c>
@@ -4246,7 +4263,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="68" spans="1:23" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:23" s="4" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A68" s="65" t="s">
         <v>252</v>
       </c>
@@ -4270,7 +4287,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="69" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:23" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A69" s="1" t="s">
         <v>68</v>
       </c>
@@ -4301,7 +4318,7 @@
       <c r="T69" s="31"/>
       <c r="U69" s="31"/>
     </row>
-    <row r="70" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
         <v>70</v>
       </c>
@@ -4333,7 +4350,7 @@
       <c r="T70" s="31"/>
       <c r="U70" s="31"/>
     </row>
-    <row r="71" spans="1:23" s="19" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:23" s="19" customFormat="1" ht="57" x14ac:dyDescent="0.45">
       <c r="A71" s="19" t="s">
         <v>244</v>
       </c>
@@ -4369,7 +4386,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="72" spans="1:23" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:23" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
         <v>189</v>
       </c>
@@ -4403,7 +4420,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="73" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
         <v>72</v>
       </c>
@@ -4462,7 +4479,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="74" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:23" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A74" s="35" t="s">
         <v>192</v>
       </c>
@@ -4491,7 +4508,7 @@
       <c r="T74" s="59"/>
       <c r="U74" s="59"/>
     </row>
-    <row r="75" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A75" s="32" t="s">
         <v>74</v>
       </c>
@@ -4524,7 +4541,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="76" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:23" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A76" s="1" t="s">
         <v>211</v>
       </c>
@@ -4555,7 +4572,7 @@
       <c r="T76" s="31"/>
       <c r="U76" s="31"/>
     </row>
-    <row r="77" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:23" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A77" s="1" t="s">
         <v>76</v>
       </c>
@@ -4587,7 +4604,7 @@
       <c r="T77" s="31"/>
       <c r="U77" s="31"/>
     </row>
-    <row r="78" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A78" s="1" t="s">
         <v>78</v>
       </c>
@@ -4646,7 +4663,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="79" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:23" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A79" s="1" t="s">
         <v>80</v>
       </c>
@@ -4678,7 +4695,7 @@
       <c r="T79" s="31"/>
       <c r="U79" s="31"/>
     </row>
-    <row r="80" spans="1:23" s="4" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:23" s="4" customFormat="1" ht="57" x14ac:dyDescent="0.45">
       <c r="A80" s="4" t="s">
         <v>83</v>
       </c>
@@ -4711,7 +4728,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="81" spans="1:23" s="4" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:23" s="4" customFormat="1" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A81" s="4" t="s">
         <v>301</v>
       </c>
@@ -4733,7 +4750,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="82" spans="1:23" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:23" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A82" s="1" t="s">
         <v>193</v>
       </c>
@@ -4768,7 +4785,7 @@
       </c>
       <c r="W82" s="4"/>
     </row>
-    <row r="83" spans="1:23" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:23" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A83" s="4" t="s">
         <v>303</v>
       </c>
@@ -4791,7 +4808,7 @@
       </c>
       <c r="W83" s="4"/>
     </row>
-    <row r="84" spans="1:23" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:23" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A84" s="4" t="s">
         <v>306</v>
       </c>
@@ -4814,7 +4831,7 @@
       </c>
       <c r="W84" s="4"/>
     </row>
-    <row r="85" spans="1:23" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:23" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A85" s="4" t="s">
         <v>309</v>
       </c>
@@ -4837,7 +4854,7 @@
       </c>
       <c r="W85" s="4"/>
     </row>
-    <row r="86" spans="1:23" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:23" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A86" s="4" t="s">
         <v>312</v>
       </c>
@@ -4860,7 +4877,7 @@
       </c>
       <c r="W86" s="4"/>
     </row>
-    <row r="87" spans="1:23" s="4" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:23" s="4" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A87" s="4" t="s">
         <v>196</v>
       </c>
@@ -4886,7 +4903,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="88" spans="1:23" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:23" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A88" s="1" t="s">
         <v>85</v>
       </c>
@@ -4951,7 +4968,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="89" spans="1:23" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:23" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A89" s="1" t="s">
         <v>87</v>
       </c>
@@ -4989,7 +5006,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="90" spans="1:23" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:23" s="4" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A90" s="4" t="s">
         <v>91</v>
       </c>
@@ -5019,7 +5036,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="91" spans="1:23" s="4" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:23" s="4" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A91" s="4" t="s">
         <v>147</v>
       </c>
@@ -5045,7 +5062,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="92" spans="1:23" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:23" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.45">
       <c r="A92" s="1" t="s">
         <v>95</v>
       </c>
@@ -5077,7 +5094,7 @@
       <c r="T92" s="31"/>
       <c r="U92" s="31"/>
     </row>
-    <row r="93" spans="1:23" s="38" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:23" s="38" customFormat="1" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A93" s="60" t="s">
         <v>314</v>
       </c>
@@ -5106,7 +5123,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="94" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:23" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A94" s="60" t="s">
         <v>218</v>
       </c>
@@ -5140,7 +5157,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="95" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:23" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A95" s="1" t="s">
         <v>149</v>
       </c>
@@ -5177,7 +5194,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="96" spans="1:23" s="26" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:23" s="26" customFormat="1" ht="57" x14ac:dyDescent="0.45">
       <c r="A96" s="26" t="s">
         <v>98</v>
       </c>
@@ -5210,7 +5227,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="97" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:23" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A97" s="4" t="s">
         <v>198</v>
       </c>
@@ -5244,7 +5261,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="98" spans="1:23" s="9" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:23" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A98" s="4" t="s">
         <v>240</v>
       </c>
@@ -5276,7 +5293,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="99" spans="1:23" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:23" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.45">
       <c r="A99" s="4" t="s">
         <v>214</v>
       </c>
@@ -5313,7 +5330,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="100" spans="1:23" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:23" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A100" s="1" t="s">
         <v>100</v>
       </c>
@@ -5344,7 +5361,7 @@
       <c r="T100" s="31"/>
       <c r="U100" s="31"/>
     </row>
-    <row r="101" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A101" s="5" t="s">
         <v>274</v>
       </c>
@@ -5368,7 +5385,7 @@
       <c r="L101" s="22"/>
       <c r="Q101" s="22"/>
     </row>
-    <row r="102" spans="1:23" s="1" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:23" s="1" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A102" s="1" t="s">
         <v>102</v>
       </c>
@@ -5406,7 +5423,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="103" spans="1:23" s="38" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:23" s="38" customFormat="1" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A103" s="61" t="s">
         <v>318</v>
       </c>
@@ -5447,7 +5464,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="104" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:23" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A104" s="1" t="s">
         <v>104</v>
       </c>
@@ -5478,7 +5495,7 @@
       <c r="T104" s="31"/>
       <c r="U104" s="31"/>
     </row>
-    <row r="105" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A105" s="1" t="s">
         <v>201</v>
       </c>
@@ -5509,7 +5526,7 @@
       <c r="T105" s="31"/>
       <c r="U105" s="31"/>
     </row>
-    <row r="106" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A106" s="1" t="s">
         <v>106</v>
       </c>
@@ -5540,7 +5557,7 @@
       <c r="T106" s="31"/>
       <c r="U106" s="31"/>
     </row>
-    <row r="107" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:23" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A107" s="1" t="s">
         <v>110</v>
       </c>
@@ -5599,7 +5616,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="108" spans="1:23" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:23" s="4" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A108" s="4" t="s">
         <v>112</v>
       </c>
@@ -5632,7 +5649,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="109" spans="1:23" s="4" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:23" s="4" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A109" s="4" t="s">
         <v>114</v>
       </c>
@@ -5662,7 +5679,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="110" spans="1:23" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:23" s="4" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>116</v>
       </c>
@@ -5694,7 +5711,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="111" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A111" s="1" t="s">
         <v>118</v>
       </c>
@@ -5747,7 +5764,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:23" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A112" s="60" t="s">
         <v>120</v>
       </c>
@@ -5800,7 +5817,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A113" s="60" t="s">
         <v>121</v>
       </c>
@@ -5844,7 +5861,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:23" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A114" s="4" t="s">
         <v>151</v>
       </c>
@@ -5877,7 +5894,7 @@
       <c r="T114" s="31"/>
       <c r="U114" s="31"/>
     </row>
-    <row r="115" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A115" s="5" t="s">
         <v>276</v>
       </c>
@@ -5910,7 +5927,7 @@
       <c r="T115"/>
       <c r="U115"/>
     </row>
-    <row r="116" spans="1:23" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:23" s="4" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A116" s="44" t="s">
         <v>123</v>
       </c>
@@ -5962,7 +5979,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="117" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A117" s="60" t="s">
         <v>126</v>
       </c>
@@ -6015,7 +6032,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A118" s="60" t="s">
         <v>232</v>
       </c>
@@ -6068,7 +6085,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A119" s="60" t="s">
         <v>129</v>
       </c>
@@ -6100,24 +6117,24 @@
       <c r="T119" s="31"/>
       <c r="U119" s="31"/>
     </row>
-    <row r="120" spans="1:23" s="71" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A120" s="74" t="s">
+    <row r="120" spans="1:23" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A120" s="72" t="s">
         <v>417</v>
       </c>
-      <c r="B120" s="74" t="s">
+      <c r="B120" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="C120" s="74" t="s">
+      <c r="C120" s="72" t="s">
         <v>418</v>
       </c>
-      <c r="D120" s="74" t="b">
-        <v>1</v>
-      </c>
-      <c r="E120" s="74" t="b">
-        <v>1</v>
-      </c>
-      <c r="F120" s="74"/>
-      <c r="G120" s="75"/>
+      <c r="D120" s="72" t="b">
+        <v>1</v>
+      </c>
+      <c r="E120" s="72" t="b">
+        <v>1</v>
+      </c>
+      <c r="F120" s="72"/>
+      <c r="G120" s="73"/>
       <c r="H120" s="45" t="s">
         <v>415</v>
       </c>
@@ -6130,34 +6147,34 @@
       <c r="K120" s="45" t="s">
         <v>415</v>
       </c>
-      <c r="L120" s="75"/>
-      <c r="M120" s="74" t="s">
+      <c r="L120" s="73"/>
+      <c r="M120" s="72" t="s">
         <v>348</v>
       </c>
-      <c r="N120" s="74" t="s">
+      <c r="N120" s="72" t="s">
         <v>348</v>
       </c>
-      <c r="O120" s="74" t="s">
+      <c r="O120" s="72" t="s">
         <v>348</v>
       </c>
-      <c r="P120" s="74" t="s">
+      <c r="P120" s="72" t="s">
         <v>348</v>
       </c>
-      <c r="Q120" s="75"/>
-      <c r="R120" s="74" t="s">
+      <c r="Q120" s="73"/>
+      <c r="R120" s="72" t="s">
         <v>360</v>
       </c>
-      <c r="S120" s="74" t="s">
+      <c r="S120" s="72" t="s">
         <v>360</v>
       </c>
-      <c r="T120" s="74" t="s">
+      <c r="T120" s="72" t="s">
         <v>360</v>
       </c>
-      <c r="U120" s="74" t="s">
+      <c r="U120" s="72" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="121" spans="1:23" s="20" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:23" s="20" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A121" s="60" t="s">
         <v>247</v>
       </c>
@@ -6196,7 +6213,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="122" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:23" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A122" s="60" t="s">
         <v>131</v>
       </c>
@@ -6237,7 +6254,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="123" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A123" s="41"/>
       <c r="B123" s="41"/>
       <c r="C123" s="41"/>
@@ -6249,7 +6266,7 @@
       <c r="M123" s="45"/>
       <c r="Q123" s="22"/>
     </row>
-    <row r="124" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A124" s="41"/>
       <c r="B124" s="41"/>
       <c r="C124" s="41"/>
@@ -6260,7 +6277,7 @@
       <c r="H124" s="39"/>
       <c r="Q124" s="22"/>
     </row>
-    <row r="125" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A125" s="41"/>
       <c r="B125" s="41"/>
       <c r="C125" s="41"/>
@@ -6271,7 +6288,7 @@
       <c r="H125" s="39"/>
       <c r="Q125" s="22"/>
     </row>
-    <row r="126" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A126" s="41"/>
       <c r="B126" s="41"/>
       <c r="C126" s="41"/>
@@ -6282,7 +6299,7 @@
       <c r="H126" s="39"/>
       <c r="Q126" s="22"/>
     </row>
-    <row r="127" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A127" s="41"/>
       <c r="B127" s="41"/>
       <c r="C127" s="41"/>
@@ -6293,7 +6310,7 @@
       <c r="H127" s="39"/>
       <c r="Q127" s="22"/>
     </row>
-    <row r="128" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A128" s="41"/>
       <c r="B128" s="41"/>
       <c r="C128" s="41"/>
@@ -6304,7 +6321,7 @@
       <c r="H128" s="39"/>
       <c r="Q128" s="22"/>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A129" s="41"/>
       <c r="B129" s="41"/>
       <c r="C129" s="41"/>
@@ -6315,7 +6332,7 @@
       <c r="H129" s="39"/>
       <c r="Q129" s="22"/>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A130" s="41"/>
       <c r="B130" s="41"/>
       <c r="C130" s="41"/>
@@ -6326,7 +6343,7 @@
       <c r="H130" s="39"/>
       <c r="Q130" s="22"/>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A131" s="41"/>
       <c r="B131" s="41"/>
       <c r="C131" s="41"/>
@@ -6337,7 +6354,7 @@
       <c r="H131" s="39"/>
       <c r="Q131" s="22"/>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A132" s="41"/>
       <c r="B132" s="41"/>
       <c r="C132" s="41"/>
@@ -6347,7 +6364,7 @@
       <c r="G132" s="48"/>
       <c r="Q132" s="22"/>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A133" s="41"/>
       <c r="B133" s="41"/>
       <c r="C133" s="41"/>
@@ -6357,7 +6374,7 @@
       <c r="G133" s="48"/>
       <c r="Q133" s="22"/>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A134" s="41"/>
       <c r="B134" s="41"/>
       <c r="C134" s="41"/>
@@ -6367,7 +6384,7 @@
       <c r="G134" s="48"/>
       <c r="Q134" s="22"/>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A135" s="41"/>
       <c r="B135" s="41"/>
       <c r="C135" s="41"/>
@@ -6377,7 +6394,7 @@
       <c r="G135" s="48"/>
       <c r="Q135" s="22"/>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A136" s="41"/>
       <c r="B136" s="41"/>
       <c r="C136" s="41"/>
@@ -6387,7 +6404,7 @@
       <c r="G136" s="48"/>
       <c r="Q136" s="22"/>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A137" s="41"/>
       <c r="B137" s="41"/>
       <c r="C137" s="41"/>
@@ -6397,7 +6414,7 @@
       <c r="G137" s="48"/>
       <c r="Q137" s="22"/>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A138" s="41"/>
       <c r="B138" s="41"/>
       <c r="C138" s="41"/>
@@ -6407,7 +6424,7 @@
       <c r="G138" s="48"/>
       <c r="Q138" s="22"/>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A139" s="41"/>
       <c r="B139" s="41"/>
       <c r="C139" s="41"/>
@@ -6417,7 +6434,7 @@
       <c r="G139" s="48"/>
       <c r="Q139" s="22"/>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A140" s="41"/>
       <c r="B140" s="41"/>
       <c r="C140" s="41"/>
@@ -6427,7 +6444,7 @@
       <c r="G140" s="48"/>
       <c r="Q140" s="22"/>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A141" s="41"/>
       <c r="B141" s="41"/>
       <c r="C141" s="41"/>
@@ -6437,7 +6454,7 @@
       <c r="G141" s="48"/>
       <c r="Q141" s="22"/>
     </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A142" s="41"/>
       <c r="B142" s="41"/>
       <c r="C142" s="41"/>
@@ -6447,7 +6464,7 @@
       <c r="G142" s="48"/>
       <c r="Q142" s="22"/>
     </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A143" s="41"/>
       <c r="B143" s="41"/>
       <c r="C143" s="41"/>
@@ -6457,7 +6474,7 @@
       <c r="G143" s="48"/>
       <c r="Q143" s="22"/>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A144" s="41"/>
       <c r="B144" s="41"/>
       <c r="C144" s="41"/>
@@ -6467,7 +6484,7 @@
       <c r="G144" s="48"/>
       <c r="Q144" s="22"/>
     </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A145" s="41"/>
       <c r="B145" s="41"/>
       <c r="C145" s="41"/>
@@ -6477,7 +6494,7 @@
       <c r="G145" s="48"/>
       <c r="Q145" s="22"/>
     </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A146" s="41"/>
       <c r="B146" s="41"/>
       <c r="C146" s="41"/>
@@ -6487,7 +6504,7 @@
       <c r="G146" s="48"/>
       <c r="Q146" s="22"/>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A147" s="41"/>
       <c r="B147" s="41"/>
       <c r="C147" s="41"/>
@@ -6497,7 +6514,7 @@
       <c r="G147" s="48"/>
       <c r="Q147" s="22"/>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A148" s="41"/>
       <c r="B148" s="41"/>
       <c r="C148" s="41"/>
@@ -6507,7 +6524,7 @@
       <c r="G148" s="48"/>
       <c r="Q148" s="22"/>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A149" s="41"/>
       <c r="B149" s="41"/>
       <c r="C149" s="41"/>
@@ -6517,7 +6534,7 @@
       <c r="G149" s="48"/>
       <c r="Q149" s="22"/>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A150" s="41"/>
       <c r="B150" s="41"/>
       <c r="C150" s="41"/>
@@ -6527,7 +6544,7 @@
       <c r="G150" s="48"/>
       <c r="Q150" s="22"/>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A151" s="41"/>
       <c r="B151" s="41"/>
       <c r="C151" s="41"/>
@@ -6537,7 +6554,7 @@
       <c r="G151" s="48"/>
       <c r="Q151" s="22"/>
     </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A152" s="41"/>
       <c r="B152" s="41"/>
       <c r="C152" s="41"/>
@@ -6547,7 +6564,7 @@
       <c r="G152" s="48"/>
       <c r="Q152" s="22"/>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A153" s="41"/>
       <c r="B153" s="41"/>
       <c r="C153" s="41"/>
@@ -6558,22 +6575,22 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="V7:V8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
     <mergeCell ref="V46:V47"/>
     <mergeCell ref="A46:A47"/>
     <mergeCell ref="B46:B47"/>
     <mergeCell ref="C46:C47"/>
     <mergeCell ref="D46:D47"/>
-    <mergeCell ref="V7:V8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="H20" r:id="rId1" display="standaarden.ondersteuning@vng.nl"/>
-    <hyperlink ref="F20" r:id="rId2"/>
-    <hyperlink ref="F45" r:id="rId3"/>
+    <hyperlink ref="H20" r:id="rId1" display="standaarden.ondersteuning@vng.nl" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F20" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F45" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="37" fitToHeight="0" orientation="landscape" r:id="rId4"/>
@@ -6581,25 +6598,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.69140625" customWidth="1"/>
-    <col min="2" max="2" width="52.23046875" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="52.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>229</v>
       </c>
@@ -6607,7 +6624,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>230</v>
       </c>
@@ -6615,8 +6632,8 @@
         <v>228</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="6" spans="1:2" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="6" spans="1:2" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A6" s="3" t="s">
         <v>208</v>
       </c>
@@ -6624,7 +6641,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:2" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A7" s="3" t="s">
         <v>209</v>
       </c>
@@ -6632,7 +6649,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:2" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A8" s="3" t="s">
         <v>210</v>
       </c>
@@ -6640,7 +6657,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.4"/>
+    <row r="9" spans="1:2" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Property nativescalars staat nu op 'no'.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/KING/props/KING.xlsx
+++ b/src/main/resources/input/KING/props/KING.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\KING\props\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\KING\Kern-taken\Imvertor\Imvertor-Maven\src\main\resources\input\KING\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38AD89AA-13E0-4169-A541-5349D454DB9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5280" windowWidth="29040" windowHeight="16440"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KING" sheetId="3" r:id="rId1"/>
@@ -1320,7 +1321,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1726,13 +1727,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
-    <cellStyle name="Explanatory Text" xfId="3" builtinId="53"/>
-    <cellStyle name="Good" xfId="4" builtinId="26"/>
+    <cellStyle name="Controlecel" xfId="1" builtinId="23"/>
+    <cellStyle name="Goed" xfId="4" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
-    <cellStyle name="Neutral 2" xfId="6"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Neutral 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Ongeldig" xfId="2" builtinId="27"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Verklarende tekst" xfId="3" builtinId="53"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2009,7 +2010,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -2020,35 +2021,35 @@
       <selection activeCell="E64" sqref="E64"/>
       <selection pane="topRight" activeCell="E64" sqref="E64"/>
       <selection pane="bottomLeft" activeCell="E64" sqref="E64"/>
-      <selection pane="bottomRight" activeCell="A76" sqref="A76:F76"/>
+      <selection pane="bottomRight" activeCell="H81" sqref="H81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.84375" customWidth="1"/>
-    <col min="2" max="2" width="20.15234375" customWidth="1"/>
-    <col min="3" max="3" width="50.69140625" customWidth="1"/>
-    <col min="4" max="4" width="10.84375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.81640625" customWidth="1"/>
+    <col min="2" max="2" width="20.1796875" customWidth="1"/>
+    <col min="3" max="3" width="50.7265625" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="2.69140625" style="18" customWidth="1"/>
-    <col min="8" max="8" width="16.61328125" customWidth="1"/>
-    <col min="9" max="9" width="14.69140625" customWidth="1"/>
-    <col min="10" max="10" width="14.3046875" customWidth="1"/>
-    <col min="11" max="11" width="15.69140625" customWidth="1"/>
-    <col min="12" max="12" width="2.3828125" style="18" customWidth="1"/>
-    <col min="13" max="13" width="18.69140625" customWidth="1"/>
-    <col min="14" max="14" width="16.07421875" customWidth="1"/>
-    <col min="15" max="16" width="15.69140625" customWidth="1"/>
-    <col min="17" max="17" width="2.3828125" style="18" customWidth="1"/>
-    <col min="18" max="18" width="19.921875" customWidth="1"/>
-    <col min="19" max="19" width="19.61328125" customWidth="1"/>
+    <col min="7" max="7" width="2.7265625" style="18" customWidth="1"/>
+    <col min="8" max="8" width="16.6328125" customWidth="1"/>
+    <col min="9" max="9" width="14.7265625" customWidth="1"/>
+    <col min="10" max="10" width="14.26953125" customWidth="1"/>
+    <col min="11" max="11" width="15.7265625" customWidth="1"/>
+    <col min="12" max="12" width="2.36328125" style="18" customWidth="1"/>
+    <col min="13" max="13" width="18.7265625" customWidth="1"/>
+    <col min="14" max="14" width="16.08984375" customWidth="1"/>
+    <col min="15" max="16" width="15.7265625" customWidth="1"/>
+    <col min="17" max="17" width="2.36328125" style="18" customWidth="1"/>
+    <col min="18" max="18" width="19.90625" customWidth="1"/>
+    <col min="19" max="19" width="19.6328125" customWidth="1"/>
     <col min="20" max="21" width="18" customWidth="1"/>
-    <col min="22" max="22" width="63.61328125" customWidth="1"/>
-    <col min="23" max="23" width="30.07421875" customWidth="1"/>
+    <col min="22" max="22" width="63.6328125" customWidth="1"/>
+    <col min="23" max="23" width="30.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="3" customFormat="1" ht="37.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:23" s="3" customFormat="1" ht="38" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2110,7 +2111,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="3" customFormat="1" ht="56.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:23" s="3" customFormat="1" ht="56.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="F2" s="57"/>
       <c r="G2" s="14"/>
       <c r="H2" s="2" t="s">
@@ -2152,7 +2153,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="3" spans="1:23" s="1" customFormat="1" ht="29.6" thickTop="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:23" s="1" customFormat="1" ht="44" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>153</v>
       </c>
@@ -2181,7 +2182,7 @@
       <c r="T3" s="31"/>
       <c r="U3" s="31"/>
     </row>
-    <row r="4" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:23" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -2212,7 +2213,7 @@
       <c r="T4" s="31"/>
       <c r="U4" s="31"/>
     </row>
-    <row r="5" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -2243,7 +2244,7 @@
       <c r="T5" s="31"/>
       <c r="U5" s="31"/>
     </row>
-    <row r="6" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>156</v>
       </c>
@@ -2264,7 +2265,7 @@
       <c r="L6" s="15"/>
       <c r="Q6" s="22"/>
     </row>
-    <row r="7" spans="1:23" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:23" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="76" t="s">
         <v>9</v>
       </c>
@@ -2299,7 +2300,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="8" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="76"/>
       <c r="B8" s="76"/>
       <c r="C8" s="76"/>
@@ -2318,7 +2319,7 @@
       <c r="U8" s="31"/>
       <c r="V8" s="75"/>
     </row>
-    <row r="9" spans="1:23" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:23" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>159</v>
       </c>
@@ -2347,7 +2348,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="10" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:23" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -2378,7 +2379,7 @@
       <c r="T10" s="31"/>
       <c r="U10" s="31"/>
     </row>
-    <row r="11" spans="1:23" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:23" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>161</v>
       </c>
@@ -2399,7 +2400,7 @@
       <c r="L11" s="15"/>
       <c r="Q11" s="22"/>
     </row>
-    <row r="12" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:23" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>134</v>
       </c>
@@ -2428,7 +2429,7 @@
       <c r="T12" s="31"/>
       <c r="U12" s="31"/>
     </row>
-    <row r="13" spans="1:23" s="8" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:23" s="8" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>237</v>
       </c>
@@ -2463,7 +2464,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="14" spans="1:23" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:23" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -2494,7 +2495,7 @@
       <c r="T14" s="31"/>
       <c r="U14" s="31"/>
     </row>
-    <row r="15" spans="1:23" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:23" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -2531,7 +2532,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="16" spans="1:23" s="1" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:23" s="1" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -2566,7 +2567,7 @@
       </c>
       <c r="W16" s="59"/>
     </row>
-    <row r="17" spans="1:23" s="1" customFormat="1" ht="17.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:23" s="1" customFormat="1" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>215</v>
       </c>
@@ -2597,7 +2598,7 @@
       <c r="T17" s="31"/>
       <c r="U17" s="31"/>
     </row>
-    <row r="18" spans="1:23" s="1" customFormat="1" ht="156.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:23" s="1" customFormat="1" ht="156.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>217</v>
       </c>
@@ -2662,7 +2663,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="19" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:23" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>163</v>
       </c>
@@ -2693,7 +2694,7 @@
       <c r="T19" s="31"/>
       <c r="U19" s="31"/>
     </row>
-    <row r="20" spans="1:23" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:23" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>136</v>
       </c>
@@ -2730,7 +2731,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="21" spans="1:23" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:23" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>139</v>
       </c>
@@ -2768,7 +2769,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="22" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:23" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>142</v>
       </c>
@@ -2805,7 +2806,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="23" spans="1:23" s="4" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:23" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A23" s="32" t="s">
         <v>25</v>
       </c>
@@ -2837,7 +2838,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="24" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>165</v>
       </c>
@@ -2866,7 +2867,7 @@
       <c r="T24" s="31"/>
       <c r="U24" s="31"/>
     </row>
-    <row r="25" spans="1:23" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:23" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
@@ -2903,7 +2904,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="26" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:23" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
@@ -2944,7 +2945,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="27" spans="1:23" s="70" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:23" s="70" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="70" t="s">
         <v>416</v>
       </c>
@@ -2979,7 +2980,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="28" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:23" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
@@ -3013,7 +3014,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="29" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:23" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>144</v>
       </c>
@@ -3047,7 +3048,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="30" spans="1:23" s="37" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:23" s="37" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>288</v>
       </c>
@@ -3072,7 +3073,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="31" spans="1:23" s="23" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:23" s="23" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>250</v>
       </c>
@@ -3107,7 +3108,7 @@
       </c>
       <c r="W31" s="50"/>
     </row>
-    <row r="32" spans="1:23" s="25" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:23" s="25" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>255</v>
       </c>
@@ -3146,7 +3147,7 @@
       </c>
       <c r="W32" s="50"/>
     </row>
-    <row r="33" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:23" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
@@ -3186,7 +3187,7 @@
       <c r="T33" s="59"/>
       <c r="U33" s="59"/>
     </row>
-    <row r="34" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:23" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>167</v>
       </c>
@@ -3217,7 +3218,7 @@
       <c r="T34" s="31"/>
       <c r="U34" s="31"/>
     </row>
-    <row r="35" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>170</v>
       </c>
@@ -3249,7 +3250,7 @@
       <c r="U35" s="31"/>
       <c r="V35" s="43"/>
     </row>
-    <row r="36" spans="1:23" s="30" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:23" s="30" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="30" t="s">
         <v>260</v>
       </c>
@@ -3278,7 +3279,7 @@
       <c r="U36" s="31"/>
       <c r="V36" s="43"/>
     </row>
-    <row r="37" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
         <v>37</v>
       </c>
@@ -3308,7 +3309,7 @@
       <c r="T37" s="31"/>
       <c r="U37" s="31"/>
     </row>
-    <row r="38" spans="1:23" s="32" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:23" s="32" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>272</v>
       </c>
@@ -3334,7 +3335,7 @@
       </c>
       <c r="W38" s="50"/>
     </row>
-    <row r="39" spans="1:23" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:23" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
@@ -3366,7 +3367,7 @@
       <c r="T39" s="31"/>
       <c r="U39" s="31"/>
     </row>
-    <row r="40" spans="1:23" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:23" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>41</v>
       </c>
@@ -3404,7 +3405,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="41" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>43</v>
       </c>
@@ -3436,7 +3437,7 @@
       <c r="T41" s="31"/>
       <c r="U41" s="31"/>
     </row>
-    <row r="42" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
         <v>254</v>
       </c>
@@ -3471,7 +3472,7 @@
       <c r="T42" s="59"/>
       <c r="U42" s="59"/>
     </row>
-    <row r="43" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:23" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>173</v>
       </c>
@@ -3511,7 +3512,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="44" spans="1:23" s="4" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:23" s="4" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A44" s="32" t="s">
         <v>45</v>
       </c>
@@ -3546,7 +3547,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="45" spans="1:23" s="4" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:23" s="4" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="44" t="s">
         <v>47</v>
       </c>
@@ -3578,7 +3579,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="46" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="76" t="s">
         <v>50</v>
       </c>
@@ -3615,7 +3616,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="47" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="76"/>
       <c r="B47" s="76"/>
       <c r="C47" s="76"/>
@@ -3634,7 +3635,7 @@
       <c r="U47" s="31"/>
       <c r="V47" s="75"/>
     </row>
-    <row r="48" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:23" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>175</v>
       </c>
@@ -3663,7 +3664,7 @@
       <c r="T48" s="31"/>
       <c r="U48" s="31"/>
     </row>
-    <row r="49" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>52</v>
       </c>
@@ -3694,7 +3695,7 @@
       <c r="T49" s="31"/>
       <c r="U49" s="31"/>
     </row>
-    <row r="50" spans="1:23" s="1" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:23" s="1" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
         <v>54</v>
       </c>
@@ -3731,7 +3732,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="51" spans="1:23" s="1" customFormat="1" ht="160.30000000000001" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:23" s="1" customFormat="1" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>213</v>
       </c>
@@ -3794,7 +3795,7 @@
       </c>
       <c r="W51"/>
     </row>
-    <row r="52" spans="1:23" s="4" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:23" s="4" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="32" t="s">
         <v>178</v>
       </c>
@@ -3820,7 +3821,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="53" spans="1:23" s="4" customFormat="1" ht="86.6" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:23" s="4" customFormat="1" ht="86.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="32" t="s">
         <v>180</v>
       </c>
@@ -3856,7 +3857,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="54" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
         <v>57</v>
       </c>
@@ -3886,7 +3887,7 @@
       <c r="U54" s="31"/>
       <c r="V54" s="43"/>
     </row>
-    <row r="55" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:23" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
         <v>59</v>
       </c>
@@ -3921,7 +3922,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="56" spans="1:23" s="4" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:23" s="4" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
         <v>61</v>
       </c>
@@ -3951,7 +3952,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="57" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:23" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="s">
         <v>183</v>
       </c>
@@ -3983,7 +3984,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="58" spans="1:23" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A58" s="65" t="s">
         <v>278</v>
       </c>
@@ -4017,7 +4018,7 @@
       </c>
       <c r="W58" s="50"/>
     </row>
-    <row r="59" spans="1:23" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:23" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="s">
         <v>280</v>
       </c>
@@ -4042,7 +4043,7 @@
       </c>
       <c r="W59" s="50"/>
     </row>
-    <row r="60" spans="1:23" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:23" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="s">
         <v>185</v>
       </c>
@@ -4065,7 +4066,7 @@
       <c r="V60" s="43"/>
       <c r="W60" s="50"/>
     </row>
-    <row r="61" spans="1:23" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:23" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A61" s="4" t="s">
         <v>283</v>
       </c>
@@ -4098,7 +4099,7 @@
       </c>
       <c r="W61" s="50"/>
     </row>
-    <row r="62" spans="1:23" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A62" s="11" t="s">
         <v>233</v>
       </c>
@@ -4137,7 +4138,7 @@
       </c>
       <c r="W62" s="50"/>
     </row>
-    <row r="63" spans="1:23" s="4" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:23" s="4" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A63" s="4" t="s">
         <v>187</v>
       </c>
@@ -4163,7 +4164,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="64" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="4" t="s">
         <v>63</v>
       </c>
@@ -4196,7 +4197,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="65" spans="1:23" s="37" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:23" s="37" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="s">
         <v>295</v>
       </c>
@@ -4224,7 +4225,7 @@
       </c>
       <c r="W65" s="61"/>
     </row>
-    <row r="66" spans="1:23" s="4" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:23" s="4" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A66" s="4" t="s">
         <v>65</v>
       </c>
@@ -4250,7 +4251,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="67" spans="1:23" s="4" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:23" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A67" s="4" t="s">
         <v>297</v>
       </c>
@@ -4271,7 +4272,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="68" spans="1:23" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:23" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A68" s="65" t="s">
         <v>252</v>
       </c>
@@ -4295,7 +4296,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="69" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:23" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>68</v>
       </c>
@@ -4326,7 +4327,7 @@
       <c r="T69" s="31"/>
       <c r="U69" s="31"/>
     </row>
-    <row r="70" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>70</v>
       </c>
@@ -4358,7 +4359,7 @@
       <c r="T70" s="31"/>
       <c r="U70" s="31"/>
     </row>
-    <row r="71" spans="1:23" s="19" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:23" s="19" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A71" s="19" t="s">
         <v>244</v>
       </c>
@@ -4394,7 +4395,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="72" spans="1:23" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:23" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>189</v>
       </c>
@@ -4428,7 +4429,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="73" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>72</v>
       </c>
@@ -4487,7 +4488,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="74" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:23" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A74" s="35" t="s">
         <v>192</v>
       </c>
@@ -4516,7 +4517,7 @@
       <c r="T74" s="59"/>
       <c r="U74" s="59"/>
     </row>
-    <row r="75" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A75" s="32" t="s">
         <v>74</v>
       </c>
@@ -4549,7 +4550,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="76" spans="1:23" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:23" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A76" s="32" t="s">
         <v>419</v>
       </c>
@@ -4566,7 +4567,7 @@
         <v>1</v>
       </c>
       <c r="F76" s="53" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G76" s="73"/>
       <c r="H76" s="32"/>
@@ -4578,7 +4579,7 @@
       <c r="V76" s="42"/>
       <c r="W76" s="73"/>
     </row>
-    <row r="77" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:23" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>211</v>
       </c>
@@ -4609,7 +4610,7 @@
       <c r="T77" s="31"/>
       <c r="U77" s="31"/>
     </row>
-    <row r="78" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:23" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>76</v>
       </c>
@@ -4641,7 +4642,7 @@
       <c r="T78" s="31"/>
       <c r="U78" s="31"/>
     </row>
-    <row r="79" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>78</v>
       </c>
@@ -4700,7 +4701,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="80" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:23" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>80</v>
       </c>
@@ -4732,7 +4733,7 @@
       <c r="T80" s="31"/>
       <c r="U80" s="31"/>
     </row>
-    <row r="81" spans="1:23" s="4" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:23" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A81" s="4" t="s">
         <v>83</v>
       </c>
@@ -4765,7 +4766,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="82" spans="1:23" s="4" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:23" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A82" s="4" t="s">
         <v>301</v>
       </c>
@@ -4787,7 +4788,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="83" spans="1:23" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:23" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>193</v>
       </c>
@@ -4822,7 +4823,7 @@
       </c>
       <c r="W83" s="4"/>
     </row>
-    <row r="84" spans="1:23" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:23" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A84" s="4" t="s">
         <v>303</v>
       </c>
@@ -4845,7 +4846,7 @@
       </c>
       <c r="W84" s="4"/>
     </row>
-    <row r="85" spans="1:23" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:23" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A85" s="4" t="s">
         <v>306</v>
       </c>
@@ -4868,7 +4869,7 @@
       </c>
       <c r="W85" s="4"/>
     </row>
-    <row r="86" spans="1:23" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:23" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A86" s="4" t="s">
         <v>309</v>
       </c>
@@ -4891,7 +4892,7 @@
       </c>
       <c r="W86" s="4"/>
     </row>
-    <row r="87" spans="1:23" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:23" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A87" s="4" t="s">
         <v>312</v>
       </c>
@@ -4914,7 +4915,7 @@
       </c>
       <c r="W87" s="4"/>
     </row>
-    <row r="88" spans="1:23" s="4" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:23" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A88" s="4" t="s">
         <v>196</v>
       </c>
@@ -4940,7 +4941,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="89" spans="1:23" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:23" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>85</v>
       </c>
@@ -5005,7 +5006,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="90" spans="1:23" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:23" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>87</v>
       </c>
@@ -5043,7 +5044,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="91" spans="1:23" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:23" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A91" s="4" t="s">
         <v>91</v>
       </c>
@@ -5073,7 +5074,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="92" spans="1:23" s="4" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:23" s="4" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="4" t="s">
         <v>147</v>
       </c>
@@ -5099,7 +5100,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="93" spans="1:23" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:23" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
         <v>95</v>
       </c>
@@ -5131,7 +5132,7 @@
       <c r="T93" s="31"/>
       <c r="U93" s="31"/>
     </row>
-    <row r="94" spans="1:23" s="38" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:23" s="38" customFormat="1" ht="116" x14ac:dyDescent="0.35">
       <c r="A94" s="60" t="s">
         <v>314</v>
       </c>
@@ -5160,7 +5161,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="95" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:23" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A95" s="60" t="s">
         <v>218</v>
       </c>
@@ -5194,7 +5195,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="96" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:23" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
         <v>149</v>
       </c>
@@ -5231,7 +5232,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="97" spans="1:23" s="26" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:23" s="26" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A97" s="26" t="s">
         <v>98</v>
       </c>
@@ -5264,7 +5265,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="98" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:23" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A98" s="4" t="s">
         <v>198</v>
       </c>
@@ -5298,7 +5299,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="99" spans="1:23" s="9" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:23" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A99" s="4" t="s">
         <v>240</v>
       </c>
@@ -5330,7 +5331,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="100" spans="1:23" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:23" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A100" s="4" t="s">
         <v>214</v>
       </c>
@@ -5367,7 +5368,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="101" spans="1:23" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:23" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
         <v>100</v>
       </c>
@@ -5398,7 +5399,7 @@
       <c r="T101" s="31"/>
       <c r="U101" s="31"/>
     </row>
-    <row r="102" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A102" s="5" t="s">
         <v>274</v>
       </c>
@@ -5422,7 +5423,7 @@
       <c r="L102" s="22"/>
       <c r="Q102" s="22"/>
     </row>
-    <row r="103" spans="1:23" s="1" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:23" s="1" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
         <v>102</v>
       </c>
@@ -5460,7 +5461,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="104" spans="1:23" s="38" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:23" s="38" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A104" s="61" t="s">
         <v>318</v>
       </c>
@@ -5501,7 +5502,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="105" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:23" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
         <v>104</v>
       </c>
@@ -5532,7 +5533,7 @@
       <c r="T105" s="31"/>
       <c r="U105" s="31"/>
     </row>
-    <row r="106" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
         <v>201</v>
       </c>
@@ -5563,7 +5564,7 @@
       <c r="T106" s="31"/>
       <c r="U106" s="31"/>
     </row>
-    <row r="107" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
         <v>106</v>
       </c>
@@ -5594,7 +5595,7 @@
       <c r="T107" s="31"/>
       <c r="U107" s="31"/>
     </row>
-    <row r="108" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:23" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
         <v>110</v>
       </c>
@@ -5653,7 +5654,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="109" spans="1:23" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:23" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A109" s="4" t="s">
         <v>112</v>
       </c>
@@ -5686,7 +5687,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="110" spans="1:23" s="4" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:23" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A110" s="4" t="s">
         <v>114</v>
       </c>
@@ -5716,7 +5717,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="111" spans="1:23" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:23" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>116</v>
       </c>
@@ -5748,7 +5749,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="112" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
         <v>118</v>
       </c>
@@ -5801,7 +5802,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:23" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A113" s="60" t="s">
         <v>120</v>
       </c>
@@ -5854,7 +5855,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A114" s="60" t="s">
         <v>121</v>
       </c>
@@ -5898,7 +5899,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:23" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A115" s="4" t="s">
         <v>151</v>
       </c>
@@ -5931,7 +5932,7 @@
       <c r="T115" s="31"/>
       <c r="U115" s="31"/>
     </row>
-    <row r="116" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A116" s="5" t="s">
         <v>276</v>
       </c>
@@ -5964,7 +5965,7 @@
       <c r="T116"/>
       <c r="U116"/>
     </row>
-    <row r="117" spans="1:23" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:23" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A117" s="44" t="s">
         <v>123</v>
       </c>
@@ -6016,7 +6017,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="118" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A118" s="60" t="s">
         <v>126</v>
       </c>
@@ -6069,7 +6070,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A119" s="60" t="s">
         <v>232</v>
       </c>
@@ -6122,7 +6123,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A120" s="60" t="s">
         <v>129</v>
       </c>
@@ -6154,7 +6155,7 @@
       <c r="T120" s="31"/>
       <c r="U120" s="31"/>
     </row>
-    <row r="121" spans="1:23" s="71" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:23" s="71" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A121" s="72" t="s">
         <v>417</v>
       </c>
@@ -6211,7 +6212,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="122" spans="1:23" s="20" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:23" s="20" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A122" s="60" t="s">
         <v>247</v>
       </c>
@@ -6250,7 +6251,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="123" spans="1:23" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:23" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A123" s="60" t="s">
         <v>131</v>
       </c>
@@ -6291,7 +6292,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="124" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A124" s="41"/>
       <c r="B124" s="41"/>
       <c r="C124" s="41"/>
@@ -6303,7 +6304,7 @@
       <c r="M124" s="45"/>
       <c r="Q124" s="22"/>
     </row>
-    <row r="125" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A125" s="41"/>
       <c r="B125" s="41"/>
       <c r="C125" s="41"/>
@@ -6314,7 +6315,7 @@
       <c r="H125" s="39"/>
       <c r="Q125" s="22"/>
     </row>
-    <row r="126" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A126" s="41"/>
       <c r="B126" s="41"/>
       <c r="C126" s="41"/>
@@ -6325,7 +6326,7 @@
       <c r="H126" s="39"/>
       <c r="Q126" s="22"/>
     </row>
-    <row r="127" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A127" s="41"/>
       <c r="B127" s="41"/>
       <c r="C127" s="41"/>
@@ -6336,7 +6337,7 @@
       <c r="H127" s="39"/>
       <c r="Q127" s="22"/>
     </row>
-    <row r="128" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A128" s="41"/>
       <c r="B128" s="41"/>
       <c r="C128" s="41"/>
@@ -6347,7 +6348,7 @@
       <c r="H128" s="39"/>
       <c r="Q128" s="22"/>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A129" s="41"/>
       <c r="B129" s="41"/>
       <c r="C129" s="41"/>
@@ -6358,7 +6359,7 @@
       <c r="H129" s="39"/>
       <c r="Q129" s="22"/>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A130" s="41"/>
       <c r="B130" s="41"/>
       <c r="C130" s="41"/>
@@ -6369,7 +6370,7 @@
       <c r="H130" s="39"/>
       <c r="Q130" s="22"/>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A131" s="41"/>
       <c r="B131" s="41"/>
       <c r="C131" s="41"/>
@@ -6380,7 +6381,7 @@
       <c r="H131" s="39"/>
       <c r="Q131" s="22"/>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A132" s="41"/>
       <c r="B132" s="41"/>
       <c r="C132" s="41"/>
@@ -6391,7 +6392,7 @@
       <c r="H132" s="39"/>
       <c r="Q132" s="22"/>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A133" s="41"/>
       <c r="B133" s="41"/>
       <c r="C133" s="41"/>
@@ -6401,7 +6402,7 @@
       <c r="G133" s="48"/>
       <c r="Q133" s="22"/>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A134" s="41"/>
       <c r="B134" s="41"/>
       <c r="C134" s="41"/>
@@ -6411,7 +6412,7 @@
       <c r="G134" s="48"/>
       <c r="Q134" s="22"/>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A135" s="41"/>
       <c r="B135" s="41"/>
       <c r="C135" s="41"/>
@@ -6421,7 +6422,7 @@
       <c r="G135" s="48"/>
       <c r="Q135" s="22"/>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A136" s="41"/>
       <c r="B136" s="41"/>
       <c r="C136" s="41"/>
@@ -6431,7 +6432,7 @@
       <c r="G136" s="48"/>
       <c r="Q136" s="22"/>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A137" s="41"/>
       <c r="B137" s="41"/>
       <c r="C137" s="41"/>
@@ -6441,7 +6442,7 @@
       <c r="G137" s="48"/>
       <c r="Q137" s="22"/>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A138" s="41"/>
       <c r="B138" s="41"/>
       <c r="C138" s="41"/>
@@ -6451,7 +6452,7 @@
       <c r="G138" s="48"/>
       <c r="Q138" s="22"/>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A139" s="41"/>
       <c r="B139" s="41"/>
       <c r="C139" s="41"/>
@@ -6461,7 +6462,7 @@
       <c r="G139" s="48"/>
       <c r="Q139" s="22"/>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A140" s="41"/>
       <c r="B140" s="41"/>
       <c r="C140" s="41"/>
@@ -6471,7 +6472,7 @@
       <c r="G140" s="48"/>
       <c r="Q140" s="22"/>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A141" s="41"/>
       <c r="B141" s="41"/>
       <c r="C141" s="41"/>
@@ -6481,7 +6482,7 @@
       <c r="G141" s="48"/>
       <c r="Q141" s="22"/>
     </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A142" s="41"/>
       <c r="B142" s="41"/>
       <c r="C142" s="41"/>
@@ -6491,7 +6492,7 @@
       <c r="G142" s="48"/>
       <c r="Q142" s="22"/>
     </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A143" s="41"/>
       <c r="B143" s="41"/>
       <c r="C143" s="41"/>
@@ -6501,7 +6502,7 @@
       <c r="G143" s="48"/>
       <c r="Q143" s="22"/>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A144" s="41"/>
       <c r="B144" s="41"/>
       <c r="C144" s="41"/>
@@ -6511,7 +6512,7 @@
       <c r="G144" s="48"/>
       <c r="Q144" s="22"/>
     </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A145" s="41"/>
       <c r="B145" s="41"/>
       <c r="C145" s="41"/>
@@ -6521,7 +6522,7 @@
       <c r="G145" s="48"/>
       <c r="Q145" s="22"/>
     </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A146" s="41"/>
       <c r="B146" s="41"/>
       <c r="C146" s="41"/>
@@ -6531,7 +6532,7 @@
       <c r="G146" s="48"/>
       <c r="Q146" s="22"/>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A147" s="41"/>
       <c r="B147" s="41"/>
       <c r="C147" s="41"/>
@@ -6541,7 +6542,7 @@
       <c r="G147" s="48"/>
       <c r="Q147" s="22"/>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A148" s="41"/>
       <c r="B148" s="41"/>
       <c r="C148" s="41"/>
@@ -6551,7 +6552,7 @@
       <c r="G148" s="48"/>
       <c r="Q148" s="22"/>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A149" s="41"/>
       <c r="B149" s="41"/>
       <c r="C149" s="41"/>
@@ -6561,7 +6562,7 @@
       <c r="G149" s="48"/>
       <c r="Q149" s="22"/>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A150" s="41"/>
       <c r="B150" s="41"/>
       <c r="C150" s="41"/>
@@ -6571,7 +6572,7 @@
       <c r="G150" s="48"/>
       <c r="Q150" s="22"/>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A151" s="41"/>
       <c r="B151" s="41"/>
       <c r="C151" s="41"/>
@@ -6581,7 +6582,7 @@
       <c r="G151" s="48"/>
       <c r="Q151" s="22"/>
     </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A152" s="41"/>
       <c r="B152" s="41"/>
       <c r="C152" s="41"/>
@@ -6591,7 +6592,7 @@
       <c r="G152" s="48"/>
       <c r="Q152" s="22"/>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A153" s="41"/>
       <c r="B153" s="41"/>
       <c r="C153" s="41"/>
@@ -6601,7 +6602,7 @@
       <c r="G153" s="48"/>
       <c r="Q153" s="22"/>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="154" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A154" s="41"/>
       <c r="B154" s="41"/>
       <c r="C154" s="41"/>
@@ -6612,22 +6613,22 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="V7:V8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
     <mergeCell ref="V46:V47"/>
     <mergeCell ref="A46:A47"/>
     <mergeCell ref="B46:B47"/>
     <mergeCell ref="C46:C47"/>
     <mergeCell ref="D46:D47"/>
-    <mergeCell ref="V7:V8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="H20" r:id="rId1" display="standaarden.ondersteuning@vng.nl"/>
-    <hyperlink ref="F20" r:id="rId2"/>
-    <hyperlink ref="F45" r:id="rId3"/>
+    <hyperlink ref="H20" r:id="rId1" display="standaarden.ondersteuning@vng.nl" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F20" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F45" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="37" fitToHeight="0" orientation="landscape" r:id="rId4"/>
@@ -6635,25 +6636,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.69140625" customWidth="1"/>
-    <col min="2" max="2" width="52.23046875" customWidth="1"/>
+    <col min="1" max="1" width="18.7265625" customWidth="1"/>
+    <col min="2" max="2" width="52.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>229</v>
       </c>
@@ -6661,7 +6662,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>230</v>
       </c>
@@ -6669,8 +6670,8 @@
         <v>228</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="6" spans="1:2" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="6" spans="1:2" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="3" t="s">
         <v>208</v>
       </c>
@@ -6678,7 +6679,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:2" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="3" t="s">
         <v>209</v>
       </c>
@@ -6686,7 +6687,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:2" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="3" t="s">
         <v>210</v>
       </c>
@@ -6694,7 +6695,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.4"/>
+    <row r="9" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Eerste aanpassingen voor Respec generatie
</commit_message>
<xml_diff>
--- a/src/main/resources/input/KING/props/KING.xlsx
+++ b/src/main/resources/input/KING/props/KING.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\KING\props\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\KING\Kern-taken\Imvertor\Imvertor-Maven\src\main\resources\input\KING\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF6E078-999C-4156-93CE-8478E6E00445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440"/>
+    <workbookView xWindow="28690" yWindow="-5440" windowWidth="51820" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KING" sheetId="3" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="427">
   <si>
     <t>Name</t>
   </si>
@@ -1331,11 +1332,15 @@
   <si>
     <t>Should a regression test be performed on the results of this run?</t>
   </si>
+  <si>
+    <t>respec
+msword</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1529,7 +1534,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1736,6 +1741,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1744,13 +1752,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
-    <cellStyle name="Explanatory Text" xfId="3" builtinId="53"/>
-    <cellStyle name="Good" xfId="4" builtinId="26"/>
+    <cellStyle name="Controlecel" xfId="1" builtinId="23"/>
+    <cellStyle name="Goed" xfId="4" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
-    <cellStyle name="Neutral 2" xfId="6"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Neutral 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Ongeldig" xfId="2" builtinId="27"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Verklarende tekst" xfId="3" builtinId="53"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2027,49 +2035,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:Z155"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="I84" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E64" sqref="E64"/>
       <selection pane="topRight" activeCell="E64" sqref="E64"/>
       <selection pane="bottomLeft" activeCell="E64" sqref="E64"/>
-      <selection pane="bottomRight" activeCell="Y93" sqref="Y93"/>
+      <selection pane="bottomRight" activeCell="I36" sqref="I36:L36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.84375" customWidth="1"/>
-    <col min="2" max="2" width="20.15234375" customWidth="1"/>
-    <col min="3" max="3" width="50.69140625" customWidth="1"/>
-    <col min="4" max="4" width="10.84375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.81640625" customWidth="1"/>
+    <col min="2" max="2" width="20.1796875" customWidth="1"/>
+    <col min="3" max="3" width="50.7265625" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="2.69140625" style="18" customWidth="1"/>
-    <col min="8" max="8" width="16.61328125" customWidth="1"/>
-    <col min="9" max="9" width="14.69140625" customWidth="1"/>
-    <col min="10" max="10" width="14.23046875" customWidth="1"/>
-    <col min="11" max="11" width="15.69140625" customWidth="1"/>
-    <col min="12" max="12" width="12.765625" customWidth="1"/>
-    <col min="13" max="13" width="2.3828125" style="18" customWidth="1"/>
-    <col min="14" max="14" width="18.69140625" customWidth="1"/>
-    <col min="15" max="15" width="16.07421875" customWidth="1"/>
-    <col min="16" max="17" width="15.69140625" customWidth="1"/>
-    <col min="18" max="18" width="12.921875" customWidth="1"/>
-    <col min="19" max="19" width="2.3828125" style="18" customWidth="1"/>
-    <col min="20" max="20" width="19.921875" customWidth="1"/>
-    <col min="21" max="21" width="19.61328125" customWidth="1"/>
+    <col min="7" max="7" width="2.7265625" style="18" customWidth="1"/>
+    <col min="8" max="8" width="16.6328125" customWidth="1"/>
+    <col min="9" max="9" width="14.7265625" customWidth="1"/>
+    <col min="10" max="10" width="14.26953125" customWidth="1"/>
+    <col min="11" max="11" width="15.7265625" customWidth="1"/>
+    <col min="12" max="12" width="12.7265625" customWidth="1"/>
+    <col min="13" max="13" width="2.36328125" style="18" customWidth="1"/>
+    <col min="14" max="14" width="18.7265625" customWidth="1"/>
+    <col min="15" max="15" width="16.08984375" customWidth="1"/>
+    <col min="16" max="17" width="15.7265625" customWidth="1"/>
+    <col min="18" max="18" width="12.90625" customWidth="1"/>
+    <col min="19" max="19" width="2.36328125" style="18" customWidth="1"/>
+    <col min="20" max="20" width="19.90625" customWidth="1"/>
+    <col min="21" max="21" width="19.6328125" customWidth="1"/>
     <col min="22" max="23" width="18" customWidth="1"/>
-    <col min="24" max="24" width="19.61328125" customWidth="1"/>
-    <col min="25" max="25" width="63.61328125" customWidth="1"/>
-    <col min="26" max="26" width="30.07421875" customWidth="1"/>
+    <col min="24" max="24" width="19.6328125" customWidth="1"/>
+    <col min="25" max="25" width="63.6328125" customWidth="1"/>
+    <col min="26" max="26" width="30.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="3" customFormat="1" ht="37.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:26" s="3" customFormat="1" ht="38" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2140,7 +2148,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="3" customFormat="1" ht="56.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:26" s="3" customFormat="1" ht="56.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="F2" s="57"/>
       <c r="G2" s="14"/>
       <c r="H2" s="2" t="s">
@@ -2191,7 +2199,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="1" customFormat="1" ht="29.6" thickTop="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:26" s="1" customFormat="1" ht="44" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>153</v>
       </c>
@@ -2223,7 +2231,7 @@
       <c r="W3" s="31"/>
       <c r="X3" s="75"/>
     </row>
-    <row r="4" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -2257,7 +2265,7 @@
       <c r="W4" s="31"/>
       <c r="X4" s="75"/>
     </row>
-    <row r="5" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -2291,7 +2299,7 @@
       <c r="W5" s="31"/>
       <c r="X5" s="75"/>
     </row>
-    <row r="6" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>156</v>
       </c>
@@ -2312,17 +2320,17 @@
       <c r="M6" s="15"/>
       <c r="S6" s="22"/>
     </row>
-    <row r="7" spans="1:26" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A7" s="77" t="s">
+    <row r="7" spans="1:26" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="77" t="s">
+      <c r="B7" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="77" t="s">
+      <c r="C7" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="77" t="b">
+      <c r="D7" s="78" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="b">
@@ -2343,18 +2351,18 @@
       <c r="V7" s="31"/>
       <c r="W7" s="31"/>
       <c r="X7" s="75"/>
-      <c r="Y7" s="76" t="s">
+      <c r="Y7" s="77" t="s">
         <v>351</v>
       </c>
       <c r="Z7" s="1" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="8" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="77"/>
-      <c r="B8" s="77"/>
-      <c r="C8" s="77"/>
-      <c r="D8" s="77"/>
+    <row r="8" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="78"/>
+      <c r="B8" s="78"/>
+      <c r="C8" s="78"/>
+      <c r="D8" s="78"/>
       <c r="F8" s="51"/>
       <c r="G8" s="15"/>
       <c r="L8" s="75"/>
@@ -2370,9 +2378,9 @@
       <c r="V8" s="31"/>
       <c r="W8" s="31"/>
       <c r="X8" s="75"/>
-      <c r="Y8" s="76"/>
-    </row>
-    <row r="9" spans="1:26" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Y8" s="77"/>
+    </row>
+    <row r="9" spans="1:26" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>159</v>
       </c>
@@ -2401,7 +2409,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="10" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -2435,7 +2443,7 @@
       <c r="W10" s="31"/>
       <c r="X10" s="75"/>
     </row>
-    <row r="11" spans="1:26" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:26" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>161</v>
       </c>
@@ -2456,7 +2464,7 @@
       <c r="M11" s="15"/>
       <c r="S11" s="22"/>
     </row>
-    <row r="12" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>134</v>
       </c>
@@ -2488,7 +2496,7 @@
       <c r="W12" s="31"/>
       <c r="X12" s="75"/>
     </row>
-    <row r="13" spans="1:26" s="8" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:26" s="8" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>237</v>
       </c>
@@ -2526,7 +2534,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="14" spans="1:26" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:26" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -2560,7 +2568,7 @@
       <c r="W14" s="31"/>
       <c r="X14" s="75"/>
     </row>
-    <row r="15" spans="1:26" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:26" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -2600,7 +2608,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="16" spans="1:26" s="1" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:26" s="1" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -2638,7 +2646,7 @@
       </c>
       <c r="Z16" s="59"/>
     </row>
-    <row r="17" spans="1:26" s="1" customFormat="1" ht="17.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:26" s="1" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>215</v>
       </c>
@@ -2672,7 +2680,7 @@
       <c r="W17" s="31"/>
       <c r="X17" s="75"/>
     </row>
-    <row r="18" spans="1:26" s="1" customFormat="1" ht="156.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:26" s="1" customFormat="1" ht="156.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>217</v>
       </c>
@@ -2746,7 +2754,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="19" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>163</v>
       </c>
@@ -2780,7 +2788,7 @@
       <c r="W19" s="31"/>
       <c r="X19" s="75"/>
     </row>
-    <row r="20" spans="1:26" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:26" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>136</v>
       </c>
@@ -2820,7 +2828,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="21" spans="1:26" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:26" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>139</v>
       </c>
@@ -2861,7 +2869,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="22" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>142</v>
       </c>
@@ -2901,7 +2909,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="23" spans="1:26" s="4" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:26" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A23" s="32" t="s">
         <v>25</v>
       </c>
@@ -2934,7 +2942,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="24" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>165</v>
       </c>
@@ -2966,7 +2974,7 @@
       <c r="W24" s="31"/>
       <c r="X24" s="75"/>
     </row>
-    <row r="25" spans="1:26" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:26" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
@@ -3006,7 +3014,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="26" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
@@ -3056,7 +3064,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="27" spans="1:26" s="70" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:26" s="70" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="70" t="s">
         <v>416</v>
       </c>
@@ -3100,7 +3108,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="28" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
@@ -3137,7 +3145,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="29" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>144</v>
       </c>
@@ -3174,7 +3182,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="30" spans="1:26" s="37" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:26" s="37" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>288</v>
       </c>
@@ -3202,7 +3210,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="31" spans="1:26" s="23" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:26" s="23" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>250</v>
       </c>
@@ -3240,7 +3248,7 @@
       </c>
       <c r="Z31" s="50"/>
     </row>
-    <row r="32" spans="1:26" s="25" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:26" s="25" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>255</v>
       </c>
@@ -3282,7 +3290,7 @@
       </c>
       <c r="Z32" s="50"/>
     </row>
-    <row r="33" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
@@ -3327,7 +3335,7 @@
       <c r="W33" s="59"/>
       <c r="X33" s="75"/>
     </row>
-    <row r="34" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>167</v>
       </c>
@@ -3361,7 +3369,7 @@
       <c r="W34" s="31"/>
       <c r="X34" s="75"/>
     </row>
-    <row r="35" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>170</v>
       </c>
@@ -3396,7 +3404,7 @@
       <c r="X35" s="45"/>
       <c r="Y35" s="43"/>
     </row>
-    <row r="36" spans="1:26" s="30" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:26" s="30" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="30" t="s">
         <v>260</v>
       </c>
@@ -3416,7 +3424,18 @@
         <v>292</v>
       </c>
       <c r="G36" s="22"/>
-      <c r="L36" s="75"/>
+      <c r="I36" s="30" t="s">
+        <v>426</v>
+      </c>
+      <c r="J36" s="76" t="s">
+        <v>426</v>
+      </c>
+      <c r="K36" s="76" t="s">
+        <v>426</v>
+      </c>
+      <c r="L36" s="76" t="s">
+        <v>426</v>
+      </c>
       <c r="M36" s="22"/>
       <c r="N36" s="38"/>
       <c r="R36" s="75"/>
@@ -3428,7 +3447,7 @@
       <c r="X36" s="45"/>
       <c r="Y36" s="43"/>
     </row>
-    <row r="37" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
         <v>37</v>
       </c>
@@ -3461,7 +3480,7 @@
       <c r="W37" s="31"/>
       <c r="X37" s="75"/>
     </row>
-    <row r="38" spans="1:26" s="32" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:26" s="32" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>272</v>
       </c>
@@ -3487,7 +3506,7 @@
       </c>
       <c r="Z38" s="50"/>
     </row>
-    <row r="39" spans="1:26" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:26" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
@@ -3522,7 +3541,7 @@
       <c r="W39" s="31"/>
       <c r="X39" s="75"/>
     </row>
-    <row r="40" spans="1:26" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:26" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>41</v>
       </c>
@@ -3563,7 +3582,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="41" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>43</v>
       </c>
@@ -3598,7 +3617,7 @@
       <c r="W41" s="31"/>
       <c r="X41" s="75"/>
     </row>
-    <row r="42" spans="1:26" s="25" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:26" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
         <v>254</v>
       </c>
@@ -3636,7 +3655,7 @@
       <c r="W42" s="59"/>
       <c r="X42" s="75"/>
     </row>
-    <row r="43" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>173</v>
       </c>
@@ -3681,7 +3700,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="44" spans="1:26" s="4" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:26" s="4" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A44" s="32" t="s">
         <v>45</v>
       </c>
@@ -3718,7 +3737,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="45" spans="1:26" s="4" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:26" s="4" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="44" t="s">
         <v>47</v>
       </c>
@@ -3752,17 +3771,17 @@
         <v>393</v>
       </c>
     </row>
-    <row r="46" spans="1:26" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="77" t="s">
+    <row r="46" spans="1:26" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="78" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="77" t="s">
+      <c r="B46" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="C46" s="77" t="s">
+      <c r="C46" s="78" t="s">
         <v>51</v>
       </c>
-      <c r="D46" s="77" t="b">
+      <c r="D46" s="78" t="b">
         <v>0</v>
       </c>
       <c r="E46" s="1" t="b">
@@ -3785,18 +3804,18 @@
       <c r="V46" s="31"/>
       <c r="W46" s="31"/>
       <c r="X46" s="45"/>
-      <c r="Y46" s="76" t="s">
+      <c r="Y46" s="77" t="s">
         <v>351</v>
       </c>
       <c r="Z46" s="1" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="47" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="77"/>
-      <c r="B47" s="77"/>
-      <c r="C47" s="77"/>
-      <c r="D47" s="77"/>
+    <row r="47" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="78"/>
+      <c r="B47" s="78"/>
+      <c r="C47" s="78"/>
+      <c r="D47" s="78"/>
       <c r="F47" s="51"/>
       <c r="G47" s="15"/>
       <c r="L47" s="75"/>
@@ -3812,9 +3831,9 @@
       <c r="V47" s="31"/>
       <c r="W47" s="31"/>
       <c r="X47" s="75"/>
-      <c r="Y47" s="76"/>
-    </row>
-    <row r="48" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y47" s="77"/>
+    </row>
+    <row r="48" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>175</v>
       </c>
@@ -3846,7 +3865,7 @@
       <c r="W48" s="31"/>
       <c r="X48" s="75"/>
     </row>
-    <row r="49" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>52</v>
       </c>
@@ -3880,7 +3899,7 @@
       <c r="W49" s="31"/>
       <c r="X49" s="75"/>
     </row>
-    <row r="50" spans="1:26" s="1" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:26" s="1" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
         <v>54</v>
       </c>
@@ -3920,7 +3939,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="51" spans="1:26" s="1" customFormat="1" ht="160.30000000000001" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:26" s="1" customFormat="1" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>213</v>
       </c>
@@ -3992,7 +4011,7 @@
       </c>
       <c r="Z51"/>
     </row>
-    <row r="52" spans="1:26" s="4" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:26" s="4" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="32" t="s">
         <v>178</v>
       </c>
@@ -4018,7 +4037,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="53" spans="1:26" s="4" customFormat="1" ht="86.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:26" s="4" customFormat="1" ht="86.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="32" t="s">
         <v>180</v>
       </c>
@@ -4057,7 +4076,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="54" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
         <v>57</v>
       </c>
@@ -4090,7 +4109,7 @@
       <c r="X54" s="75"/>
       <c r="Y54" s="43"/>
     </row>
-    <row r="55" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
         <v>59</v>
       </c>
@@ -4128,7 +4147,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="56" spans="1:26" s="4" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:26" s="4" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
         <v>61</v>
       </c>
@@ -4160,7 +4179,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="57" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="s">
         <v>183</v>
       </c>
@@ -4195,7 +4214,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="58" spans="1:26" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:26" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A58" s="65" t="s">
         <v>278</v>
       </c>
@@ -4232,7 +4251,7 @@
       </c>
       <c r="Z58" s="50"/>
     </row>
-    <row r="59" spans="1:26" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:26" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="s">
         <v>280</v>
       </c>
@@ -4257,7 +4276,7 @@
       </c>
       <c r="Z59" s="50"/>
     </row>
-    <row r="60" spans="1:26" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:26" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="s">
         <v>185</v>
       </c>
@@ -4280,7 +4299,7 @@
       <c r="Y60" s="43"/>
       <c r="Z60" s="50"/>
     </row>
-    <row r="61" spans="1:26" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:26" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A61" s="4" t="s">
         <v>283</v>
       </c>
@@ -4315,7 +4334,7 @@
       </c>
       <c r="Z61" s="50"/>
     </row>
-    <row r="62" spans="1:26" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:26" ht="29" x14ac:dyDescent="0.35">
       <c r="A62" s="11" t="s">
         <v>233</v>
       </c>
@@ -4357,7 +4376,7 @@
       </c>
       <c r="Z62" s="50"/>
     </row>
-    <row r="63" spans="1:26" s="4" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:26" s="4" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A63" s="4" t="s">
         <v>187</v>
       </c>
@@ -4383,7 +4402,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="64" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="4" t="s">
         <v>63</v>
       </c>
@@ -4419,7 +4438,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="65" spans="1:26" s="37" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:26" s="37" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="s">
         <v>295</v>
       </c>
@@ -4450,7 +4469,7 @@
       </c>
       <c r="Z65" s="61"/>
     </row>
-    <row r="66" spans="1:26" s="4" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:26" s="4" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A66" s="4" t="s">
         <v>65</v>
       </c>
@@ -4476,7 +4495,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="67" spans="1:26" s="4" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:26" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A67" s="4" t="s">
         <v>297</v>
       </c>
@@ -4497,7 +4516,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="68" spans="1:26" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:26" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A68" s="65" t="s">
         <v>252</v>
       </c>
@@ -4521,7 +4540,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="69" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>68</v>
       </c>
@@ -4555,7 +4574,7 @@
       <c r="W69" s="31"/>
       <c r="X69" s="75"/>
     </row>
-    <row r="70" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>70</v>
       </c>
@@ -4590,7 +4609,7 @@
       <c r="W70" s="31"/>
       <c r="X70" s="45"/>
     </row>
-    <row r="71" spans="1:26" s="19" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:26" s="19" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A71" s="19" t="s">
         <v>244</v>
       </c>
@@ -4629,7 +4648,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="72" spans="1:26" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:26" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>189</v>
       </c>
@@ -4666,7 +4685,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="73" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>72</v>
       </c>
@@ -4734,7 +4753,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="74" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A74" s="35" t="s">
         <v>192</v>
       </c>
@@ -4766,7 +4785,7 @@
       <c r="W74" s="59"/>
       <c r="X74" s="75"/>
     </row>
-    <row r="75" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A75" s="32" t="s">
         <v>74</v>
       </c>
@@ -4801,7 +4820,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="76" spans="1:26" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:26" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A76" s="32" t="s">
         <v>419</v>
       </c>
@@ -4832,7 +4851,7 @@
       <c r="Y76" s="42"/>
       <c r="Z76" s="73"/>
     </row>
-    <row r="77" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>211</v>
       </c>
@@ -4866,7 +4885,7 @@
       <c r="W77" s="31"/>
       <c r="X77" s="75"/>
     </row>
-    <row r="78" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>76</v>
       </c>
@@ -4901,7 +4920,7 @@
       <c r="W78" s="31"/>
       <c r="X78" s="32"/>
     </row>
-    <row r="79" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>78</v>
       </c>
@@ -4969,7 +4988,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="80" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>80</v>
       </c>
@@ -5004,7 +5023,7 @@
       <c r="W80" s="31"/>
       <c r="X80" s="45"/>
     </row>
-    <row r="81" spans="1:26" s="4" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:26" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A81" s="4" t="s">
         <v>83</v>
       </c>
@@ -5039,7 +5058,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="82" spans="1:26" s="4" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:26" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A82" s="4" t="s">
         <v>301</v>
       </c>
@@ -5061,7 +5080,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="83" spans="1:26" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:26" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>193</v>
       </c>
@@ -5099,7 +5118,7 @@
       </c>
       <c r="Z83" s="4"/>
     </row>
-    <row r="84" spans="1:26" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:26" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A84" s="4" t="s">
         <v>303</v>
       </c>
@@ -5122,7 +5141,7 @@
       </c>
       <c r="Z84" s="4"/>
     </row>
-    <row r="85" spans="1:26" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:26" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A85" s="4" t="s">
         <v>306</v>
       </c>
@@ -5145,7 +5164,7 @@
       </c>
       <c r="Z85" s="4"/>
     </row>
-    <row r="86" spans="1:26" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:26" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A86" s="4" t="s">
         <v>309</v>
       </c>
@@ -5168,7 +5187,7 @@
       </c>
       <c r="Z86" s="4"/>
     </row>
-    <row r="87" spans="1:26" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:26" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A87" s="4" t="s">
         <v>312</v>
       </c>
@@ -5191,7 +5210,7 @@
       </c>
       <c r="Z87" s="4"/>
     </row>
-    <row r="88" spans="1:26" s="4" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:26" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A88" s="4" t="s">
         <v>196</v>
       </c>
@@ -5217,7 +5236,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="89" spans="1:26" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:26" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>85</v>
       </c>
@@ -5291,7 +5310,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="90" spans="1:26" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:26" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>87</v>
       </c>
@@ -5332,7 +5351,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="91" spans="1:26" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:26" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A91" s="4" t="s">
         <v>91</v>
       </c>
@@ -5364,7 +5383,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="92" spans="1:26" s="4" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:26" s="4" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="4" t="s">
         <v>147</v>
       </c>
@@ -5390,7 +5409,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="93" spans="1:26" s="4" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:26" s="4" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="32" t="s">
         <v>424</v>
       </c>
@@ -5423,7 +5442,7 @@
       </c>
       <c r="Y93" s="58"/>
     </row>
-    <row r="94" spans="1:26" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:26" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
         <v>95</v>
       </c>
@@ -5458,7 +5477,7 @@
       <c r="W94" s="31"/>
       <c r="X94" s="45"/>
     </row>
-    <row r="95" spans="1:26" s="38" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:26" s="38" customFormat="1" ht="116" x14ac:dyDescent="0.35">
       <c r="A95" s="60" t="s">
         <v>314</v>
       </c>
@@ -5490,7 +5509,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="96" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:26" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A96" s="60" t="s">
         <v>218</v>
       </c>
@@ -5527,7 +5546,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="97" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
         <v>149</v>
       </c>
@@ -5567,7 +5586,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="98" spans="1:26" s="26" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:26" s="26" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A98" s="26" t="s">
         <v>98</v>
       </c>
@@ -5603,7 +5622,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="99" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A99" s="4" t="s">
         <v>198</v>
       </c>
@@ -5640,7 +5659,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="100" spans="1:26" s="9" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:26" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A100" s="4" t="s">
         <v>240</v>
       </c>
@@ -5675,7 +5694,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="101" spans="1:26" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:26" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A101" s="4" t="s">
         <v>214</v>
       </c>
@@ -5715,7 +5734,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="102" spans="1:26" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:26" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
         <v>100</v>
       </c>
@@ -5749,7 +5768,7 @@
       <c r="W102" s="31"/>
       <c r="X102" s="75"/>
     </row>
-    <row r="103" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A103" s="5" t="s">
         <v>274</v>
       </c>
@@ -5773,7 +5792,7 @@
       <c r="M103" s="22"/>
       <c r="S103" s="22"/>
     </row>
-    <row r="104" spans="1:26" s="1" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:26" s="1" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
         <v>102</v>
       </c>
@@ -5814,7 +5833,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="105" spans="1:26" s="38" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:26" s="38" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A105" s="61" t="s">
         <v>318</v>
       </c>
@@ -5858,7 +5877,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="106" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
         <v>104</v>
       </c>
@@ -5892,7 +5911,7 @@
       <c r="W106" s="31"/>
       <c r="X106" s="75"/>
     </row>
-    <row r="107" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
         <v>201</v>
       </c>
@@ -5926,7 +5945,7 @@
       <c r="W107" s="31"/>
       <c r="X107" s="75"/>
     </row>
-    <row r="108" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
         <v>106</v>
       </c>
@@ -5960,7 +5979,7 @@
       <c r="W108" s="31"/>
       <c r="X108" s="75"/>
     </row>
-    <row r="109" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
         <v>110</v>
       </c>
@@ -6028,7 +6047,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="110" spans="1:26" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:26" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A110" s="4" t="s">
         <v>112</v>
       </c>
@@ -6063,7 +6082,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="111" spans="1:26" s="4" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:26" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A111" s="4" t="s">
         <v>114</v>
       </c>
@@ -6093,7 +6112,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="112" spans="1:26" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:26" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>116</v>
       </c>
@@ -6126,7 +6145,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="113" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
         <v>118</v>
       </c>
@@ -6188,7 +6207,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A114" s="60" t="s">
         <v>120</v>
       </c>
@@ -6250,7 +6269,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A115" s="60" t="s">
         <v>121</v>
       </c>
@@ -6301,7 +6320,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A116" s="4" t="s">
         <v>151</v>
       </c>
@@ -6337,7 +6356,7 @@
       <c r="W116" s="31"/>
       <c r="X116" s="75"/>
     </row>
-    <row r="117" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A117" s="5" t="s">
         <v>276</v>
       </c>
@@ -6373,7 +6392,7 @@
       <c r="W117"/>
       <c r="X117"/>
     </row>
-    <row r="118" spans="1:26" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:26" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A118" s="44" t="s">
         <v>123</v>
       </c>
@@ -6434,7 +6453,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="119" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A119" s="60" t="s">
         <v>126</v>
       </c>
@@ -6496,7 +6515,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A120" s="60" t="s">
         <v>232</v>
       </c>
@@ -6558,7 +6577,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="121" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A121" s="60" t="s">
         <v>129</v>
       </c>
@@ -6593,7 +6612,7 @@
       <c r="W121" s="31"/>
       <c r="X121" s="45"/>
     </row>
-    <row r="122" spans="1:26" s="71" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:26" s="71" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A122" s="72" t="s">
         <v>417</v>
       </c>
@@ -6659,7 +6678,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="123" spans="1:26" s="20" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:26" s="20" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A123" s="60" t="s">
         <v>247</v>
       </c>
@@ -6701,7 +6720,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="124" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A124" s="60" t="s">
         <v>131</v>
       </c>
@@ -6745,7 +6764,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="125" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A125" s="41"/>
       <c r="B125" s="41"/>
       <c r="C125" s="41"/>
@@ -6757,7 +6776,7 @@
       <c r="N125" s="45"/>
       <c r="S125" s="22"/>
     </row>
-    <row r="126" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A126" s="41"/>
       <c r="B126" s="41"/>
       <c r="C126" s="41"/>
@@ -6768,7 +6787,7 @@
       <c r="H126" s="39"/>
       <c r="S126" s="22"/>
     </row>
-    <row r="127" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A127" s="41"/>
       <c r="B127" s="41"/>
       <c r="C127" s="41"/>
@@ -6779,7 +6798,7 @@
       <c r="H127" s="39"/>
       <c r="S127" s="22"/>
     </row>
-    <row r="128" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A128" s="41"/>
       <c r="B128" s="41"/>
       <c r="C128" s="41"/>
@@ -6790,7 +6809,7 @@
       <c r="H128" s="39"/>
       <c r="S128" s="22"/>
     </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A129" s="41"/>
       <c r="B129" s="41"/>
       <c r="C129" s="41"/>
@@ -6801,7 +6820,7 @@
       <c r="H129" s="39"/>
       <c r="S129" s="22"/>
     </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A130" s="41"/>
       <c r="B130" s="41"/>
       <c r="C130" s="41"/>
@@ -6812,7 +6831,7 @@
       <c r="H130" s="39"/>
       <c r="S130" s="22"/>
     </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A131" s="41"/>
       <c r="B131" s="41"/>
       <c r="C131" s="41"/>
@@ -6823,7 +6842,7 @@
       <c r="H131" s="39"/>
       <c r="S131" s="22"/>
     </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="132" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A132" s="41"/>
       <c r="B132" s="41"/>
       <c r="C132" s="41"/>
@@ -6834,7 +6853,7 @@
       <c r="H132" s="39"/>
       <c r="S132" s="22"/>
     </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A133" s="41"/>
       <c r="B133" s="41"/>
       <c r="C133" s="41"/>
@@ -6845,7 +6864,7 @@
       <c r="H133" s="39"/>
       <c r="S133" s="22"/>
     </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A134" s="41"/>
       <c r="B134" s="41"/>
       <c r="C134" s="41"/>
@@ -6855,7 +6874,7 @@
       <c r="G134" s="48"/>
       <c r="S134" s="22"/>
     </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A135" s="41"/>
       <c r="B135" s="41"/>
       <c r="C135" s="41"/>
@@ -6865,7 +6884,7 @@
       <c r="G135" s="48"/>
       <c r="S135" s="22"/>
     </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A136" s="41"/>
       <c r="B136" s="41"/>
       <c r="C136" s="41"/>
@@ -6875,7 +6894,7 @@
       <c r="G136" s="48"/>
       <c r="S136" s="22"/>
     </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A137" s="41"/>
       <c r="B137" s="41"/>
       <c r="C137" s="41"/>
@@ -6885,7 +6904,7 @@
       <c r="G137" s="48"/>
       <c r="S137" s="22"/>
     </row>
-    <row r="138" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A138" s="41"/>
       <c r="B138" s="41"/>
       <c r="C138" s="41"/>
@@ -6895,7 +6914,7 @@
       <c r="G138" s="48"/>
       <c r="S138" s="22"/>
     </row>
-    <row r="139" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A139" s="41"/>
       <c r="B139" s="41"/>
       <c r="C139" s="41"/>
@@ -6905,7 +6924,7 @@
       <c r="G139" s="48"/>
       <c r="S139" s="22"/>
     </row>
-    <row r="140" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A140" s="41"/>
       <c r="B140" s="41"/>
       <c r="C140" s="41"/>
@@ -6915,7 +6934,7 @@
       <c r="G140" s="48"/>
       <c r="S140" s="22"/>
     </row>
-    <row r="141" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A141" s="41"/>
       <c r="B141" s="41"/>
       <c r="C141" s="41"/>
@@ -6925,7 +6944,7 @@
       <c r="G141" s="48"/>
       <c r="S141" s="22"/>
     </row>
-    <row r="142" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A142" s="41"/>
       <c r="B142" s="41"/>
       <c r="C142" s="41"/>
@@ -6935,7 +6954,7 @@
       <c r="G142" s="48"/>
       <c r="S142" s="22"/>
     </row>
-    <row r="143" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A143" s="41"/>
       <c r="B143" s="41"/>
       <c r="C143" s="41"/>
@@ -6945,7 +6964,7 @@
       <c r="G143" s="48"/>
       <c r="S143" s="22"/>
     </row>
-    <row r="144" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A144" s="41"/>
       <c r="B144" s="41"/>
       <c r="C144" s="41"/>
@@ -6955,7 +6974,7 @@
       <c r="G144" s="48"/>
       <c r="S144" s="22"/>
     </row>
-    <row r="145" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A145" s="41"/>
       <c r="B145" s="41"/>
       <c r="C145" s="41"/>
@@ -6965,7 +6984,7 @@
       <c r="G145" s="48"/>
       <c r="S145" s="22"/>
     </row>
-    <row r="146" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A146" s="41"/>
       <c r="B146" s="41"/>
       <c r="C146" s="41"/>
@@ -6975,7 +6994,7 @@
       <c r="G146" s="48"/>
       <c r="S146" s="22"/>
     </row>
-    <row r="147" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A147" s="41"/>
       <c r="B147" s="41"/>
       <c r="C147" s="41"/>
@@ -6985,7 +7004,7 @@
       <c r="G147" s="48"/>
       <c r="S147" s="22"/>
     </row>
-    <row r="148" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A148" s="41"/>
       <c r="B148" s="41"/>
       <c r="C148" s="41"/>
@@ -6995,7 +7014,7 @@
       <c r="G148" s="48"/>
       <c r="S148" s="22"/>
     </row>
-    <row r="149" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A149" s="41"/>
       <c r="B149" s="41"/>
       <c r="C149" s="41"/>
@@ -7005,7 +7024,7 @@
       <c r="G149" s="48"/>
       <c r="S149" s="22"/>
     </row>
-    <row r="150" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A150" s="41"/>
       <c r="B150" s="41"/>
       <c r="C150" s="41"/>
@@ -7015,7 +7034,7 @@
       <c r="G150" s="48"/>
       <c r="S150" s="22"/>
     </row>
-    <row r="151" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A151" s="41"/>
       <c r="B151" s="41"/>
       <c r="C151" s="41"/>
@@ -7025,7 +7044,7 @@
       <c r="G151" s="48"/>
       <c r="S151" s="22"/>
     </row>
-    <row r="152" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A152" s="41"/>
       <c r="B152" s="41"/>
       <c r="C152" s="41"/>
@@ -7035,7 +7054,7 @@
       <c r="G152" s="48"/>
       <c r="S152" s="22"/>
     </row>
-    <row r="153" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A153" s="41"/>
       <c r="B153" s="41"/>
       <c r="C153" s="41"/>
@@ -7045,7 +7064,7 @@
       <c r="G153" s="48"/>
       <c r="S153" s="22"/>
     </row>
-    <row r="154" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="154" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A154" s="41"/>
       <c r="B154" s="41"/>
       <c r="C154" s="41"/>
@@ -7055,7 +7074,7 @@
       <c r="G154" s="48"/>
       <c r="S154" s="22"/>
     </row>
-    <row r="155" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="155" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A155" s="41"/>
       <c r="B155" s="41"/>
       <c r="C155" s="41"/>
@@ -7066,22 +7085,22 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="Y46:Y47"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
     <mergeCell ref="Y7:Y8"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="Y46:Y47"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="H20" r:id="rId1" display="standaarden.ondersteuning@vng.nl"/>
-    <hyperlink ref="F20" r:id="rId2"/>
-    <hyperlink ref="F45" r:id="rId3"/>
+    <hyperlink ref="H20" r:id="rId1" display="standaarden.ondersteuning@vng.nl" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F20" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F45" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="37" fitToHeight="0" orientation="landscape" r:id="rId4"/>
@@ -7089,25 +7108,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.69140625" customWidth="1"/>
-    <col min="2" max="2" width="52.23046875" customWidth="1"/>
+    <col min="1" max="1" width="18.7265625" customWidth="1"/>
+    <col min="2" max="2" width="52.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>229</v>
       </c>
@@ -7115,7 +7134,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>230</v>
       </c>
@@ -7123,8 +7142,8 @@
         <v>228</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="6" spans="1:2" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="6" spans="1:2" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="3" t="s">
         <v>208</v>
       </c>
@@ -7132,7 +7151,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:2" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="3" t="s">
         <v>209</v>
       </c>
@@ -7140,7 +7159,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:2" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="3" t="s">
         <v>210</v>
       </c>
@@ -7148,7 +7167,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.4"/>
+    <row r="9" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
T.b.v. onderzoek naar het genereren van Respec.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/KING/props/KING.xlsx
+++ b/src/main/resources/input/KING/props/KING.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\KING\Kern-taken\Imvertor\Imvertor-Maven\src\main\resources\input\KING\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF6E078-999C-4156-93CE-8478E6E00445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8589F725-48B2-4F2E-B4A0-ED2FB46F09BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28690" yWindow="-5440" windowWidth="51820" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1333,8 +1333,7 @@
     <t>Should a regression test be performed on the results of this run?</t>
   </si>
   <si>
-    <t>respec
-msword</t>
+    <t>respec</t>
   </si>
 </sst>
 </file>
@@ -2046,7 +2045,7 @@
       <selection activeCell="E64" sqref="E64"/>
       <selection pane="topRight" activeCell="E64" sqref="E64"/>
       <selection pane="bottomLeft" activeCell="E64" sqref="E64"/>
-      <selection pane="bottomRight" activeCell="I36" sqref="I36:L36"/>
+      <selection pane="bottomRight" activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7085,16 +7084,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="Y7:Y8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
     <mergeCell ref="Y46:Y47"/>
     <mergeCell ref="A46:A47"/>
     <mergeCell ref="B46:B47"/>
     <mergeCell ref="C46:C47"/>
     <mergeCell ref="D46:D47"/>
-    <mergeCell ref="Y7:Y8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Commentaar geplaatst bij createoffice, createofficeanchor en createofficevariant.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/KING/props/KING.xlsx
+++ b/src/main/resources/input/KING/props/KING.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\KING\props\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\KING\Kern-taken\Imvertor\Imvertor-Maven\src\main\resources\input\KING\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA3D489-4035-4CA9-82A9-5700E8B50709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440"/>
+    <workbookView xWindow="28690" yWindow="-5440" windowWidth="51820" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KING" sheetId="3" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="429">
   <si>
     <t>Name</t>
   </si>
@@ -1331,11 +1332,20 @@
   <si>
     <t>Should a regression test be performed on the results of this run?</t>
   </si>
+  <si>
+    <t>Het lijkt er op dat je helemaal niet meerdere formats kunt definiëren gescheiden door een spatie. Alleen het eerste type dat gedefinieerd wordt, wordt gegenereerd.</t>
+  </si>
+  <si>
+    <t>De 'doc' optie lijkt nog niet geïmplementeerd.</t>
+  </si>
+  <si>
+    <t>Het maakt voor het formaat niet uit welke variant je specificeert, 'id' of 'name'.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1744,13 +1754,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
-    <cellStyle name="Explanatory Text" xfId="3" builtinId="53"/>
-    <cellStyle name="Good" xfId="4" builtinId="26"/>
+    <cellStyle name="Controlecel" xfId="1" builtinId="23"/>
+    <cellStyle name="Goed" xfId="4" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
-    <cellStyle name="Neutral 2" xfId="6"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Neutral 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Ongeldig" xfId="2" builtinId="27"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Verklarende tekst" xfId="3" builtinId="53"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2027,49 +2037,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:Z155"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="I84" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E64" sqref="E64"/>
       <selection pane="topRight" activeCell="E64" sqref="E64"/>
       <selection pane="bottomLeft" activeCell="E64" sqref="E64"/>
-      <selection pane="bottomRight" activeCell="Y93" sqref="Y93"/>
+      <selection pane="bottomRight" activeCell="Y34" sqref="Y34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.84375" customWidth="1"/>
-    <col min="2" max="2" width="20.15234375" customWidth="1"/>
-    <col min="3" max="3" width="50.69140625" customWidth="1"/>
-    <col min="4" max="4" width="10.84375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.81640625" customWidth="1"/>
+    <col min="2" max="2" width="20.1796875" customWidth="1"/>
+    <col min="3" max="3" width="50.7265625" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="2.69140625" style="18" customWidth="1"/>
-    <col min="8" max="8" width="16.61328125" customWidth="1"/>
-    <col min="9" max="9" width="14.69140625" customWidth="1"/>
-    <col min="10" max="10" width="14.23046875" customWidth="1"/>
-    <col min="11" max="11" width="15.69140625" customWidth="1"/>
-    <col min="12" max="12" width="12.765625" customWidth="1"/>
-    <col min="13" max="13" width="2.3828125" style="18" customWidth="1"/>
-    <col min="14" max="14" width="18.69140625" customWidth="1"/>
-    <col min="15" max="15" width="16.07421875" customWidth="1"/>
-    <col min="16" max="17" width="15.69140625" customWidth="1"/>
-    <col min="18" max="18" width="12.921875" customWidth="1"/>
-    <col min="19" max="19" width="2.3828125" style="18" customWidth="1"/>
-    <col min="20" max="20" width="19.921875" customWidth="1"/>
-    <col min="21" max="21" width="19.61328125" customWidth="1"/>
+    <col min="7" max="7" width="2.7265625" style="18" customWidth="1"/>
+    <col min="8" max="8" width="16.6328125" customWidth="1"/>
+    <col min="9" max="9" width="14.7265625" customWidth="1"/>
+    <col min="10" max="10" width="14.26953125" customWidth="1"/>
+    <col min="11" max="11" width="15.7265625" customWidth="1"/>
+    <col min="12" max="12" width="12.7265625" customWidth="1"/>
+    <col min="13" max="13" width="2.36328125" style="18" customWidth="1"/>
+    <col min="14" max="14" width="18.7265625" customWidth="1"/>
+    <col min="15" max="15" width="16.08984375" customWidth="1"/>
+    <col min="16" max="17" width="15.7265625" customWidth="1"/>
+    <col min="18" max="18" width="12.90625" customWidth="1"/>
+    <col min="19" max="19" width="2.36328125" style="18" customWidth="1"/>
+    <col min="20" max="20" width="19.90625" customWidth="1"/>
+    <col min="21" max="21" width="19.6328125" customWidth="1"/>
     <col min="22" max="23" width="18" customWidth="1"/>
-    <col min="24" max="24" width="19.61328125" customWidth="1"/>
-    <col min="25" max="25" width="63.61328125" customWidth="1"/>
-    <col min="26" max="26" width="30.07421875" customWidth="1"/>
+    <col min="24" max="24" width="19.6328125" customWidth="1"/>
+    <col min="25" max="25" width="63.6328125" customWidth="1"/>
+    <col min="26" max="26" width="30.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="3" customFormat="1" ht="37.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:26" s="3" customFormat="1" ht="38" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2140,7 +2150,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="3" customFormat="1" ht="56.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:26" s="3" customFormat="1" ht="56.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="F2" s="57"/>
       <c r="G2" s="14"/>
       <c r="H2" s="2" t="s">
@@ -2191,7 +2201,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="1" customFormat="1" ht="29.6" thickTop="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:26" s="1" customFormat="1" ht="44" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>153</v>
       </c>
@@ -2223,7 +2233,7 @@
       <c r="W3" s="31"/>
       <c r="X3" s="75"/>
     </row>
-    <row r="4" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -2257,7 +2267,7 @@
       <c r="W4" s="31"/>
       <c r="X4" s="75"/>
     </row>
-    <row r="5" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -2291,7 +2301,7 @@
       <c r="W5" s="31"/>
       <c r="X5" s="75"/>
     </row>
-    <row r="6" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>156</v>
       </c>
@@ -2312,7 +2322,7 @@
       <c r="M6" s="15"/>
       <c r="S6" s="22"/>
     </row>
-    <row r="7" spans="1:26" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:26" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="77" t="s">
         <v>9</v>
       </c>
@@ -2350,7 +2360,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="8" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="77"/>
       <c r="B8" s="77"/>
       <c r="C8" s="77"/>
@@ -2372,7 +2382,7 @@
       <c r="X8" s="75"/>
       <c r="Y8" s="76"/>
     </row>
-    <row r="9" spans="1:26" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:26" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>159</v>
       </c>
@@ -2401,7 +2411,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="10" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -2435,7 +2445,7 @@
       <c r="W10" s="31"/>
       <c r="X10" s="75"/>
     </row>
-    <row r="11" spans="1:26" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:26" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>161</v>
       </c>
@@ -2456,7 +2466,7 @@
       <c r="M11" s="15"/>
       <c r="S11" s="22"/>
     </row>
-    <row r="12" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>134</v>
       </c>
@@ -2488,7 +2498,7 @@
       <c r="W12" s="31"/>
       <c r="X12" s="75"/>
     </row>
-    <row r="13" spans="1:26" s="8" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:26" s="8" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>237</v>
       </c>
@@ -2526,7 +2536,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="14" spans="1:26" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:26" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -2560,7 +2570,7 @@
       <c r="W14" s="31"/>
       <c r="X14" s="75"/>
     </row>
-    <row r="15" spans="1:26" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:26" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -2600,7 +2610,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="16" spans="1:26" s="1" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:26" s="1" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -2638,7 +2648,7 @@
       </c>
       <c r="Z16" s="59"/>
     </row>
-    <row r="17" spans="1:26" s="1" customFormat="1" ht="17.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:26" s="1" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>215</v>
       </c>
@@ -2672,7 +2682,7 @@
       <c r="W17" s="31"/>
       <c r="X17" s="75"/>
     </row>
-    <row r="18" spans="1:26" s="1" customFormat="1" ht="156.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:26" s="1" customFormat="1" ht="156.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>217</v>
       </c>
@@ -2746,7 +2756,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="19" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>163</v>
       </c>
@@ -2780,7 +2790,7 @@
       <c r="W19" s="31"/>
       <c r="X19" s="75"/>
     </row>
-    <row r="20" spans="1:26" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:26" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>136</v>
       </c>
@@ -2820,7 +2830,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="21" spans="1:26" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:26" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>139</v>
       </c>
@@ -2861,7 +2871,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="22" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>142</v>
       </c>
@@ -2901,7 +2911,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="23" spans="1:26" s="4" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:26" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A23" s="32" t="s">
         <v>25</v>
       </c>
@@ -2934,7 +2944,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="24" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>165</v>
       </c>
@@ -2966,7 +2976,7 @@
       <c r="W24" s="31"/>
       <c r="X24" s="75"/>
     </row>
-    <row r="25" spans="1:26" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:26" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
@@ -3006,7 +3016,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="26" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
@@ -3056,7 +3066,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="27" spans="1:26" s="70" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:26" s="70" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="70" t="s">
         <v>416</v>
       </c>
@@ -3100,7 +3110,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="28" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
@@ -3137,7 +3147,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="29" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>144</v>
       </c>
@@ -3174,7 +3184,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="30" spans="1:26" s="37" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:26" s="37" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>288</v>
       </c>
@@ -3202,7 +3212,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="31" spans="1:26" s="23" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:26" s="23" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>250</v>
       </c>
@@ -3240,7 +3250,7 @@
       </c>
       <c r="Z31" s="50"/>
     </row>
-    <row r="32" spans="1:26" s="25" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:26" s="25" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>255</v>
       </c>
@@ -3282,7 +3292,7 @@
       </c>
       <c r="Z32" s="50"/>
     </row>
-    <row r="33" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
@@ -3326,8 +3336,11 @@
       <c r="V33" s="59"/>
       <c r="W33" s="59"/>
       <c r="X33" s="75"/>
-    </row>
-    <row r="34" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y33" s="58" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>167</v>
       </c>
@@ -3360,8 +3373,11 @@
       <c r="V34" s="31"/>
       <c r="W34" s="31"/>
       <c r="X34" s="75"/>
-    </row>
-    <row r="35" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y34" s="58" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>170</v>
       </c>
@@ -3396,7 +3412,7 @@
       <c r="X35" s="45"/>
       <c r="Y35" s="43"/>
     </row>
-    <row r="36" spans="1:26" s="30" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:26" s="30" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A36" s="30" t="s">
         <v>260</v>
       </c>
@@ -3426,9 +3442,11 @@
       <c r="V36" s="31"/>
       <c r="W36" s="31"/>
       <c r="X36" s="45"/>
-      <c r="Y36" s="43"/>
-    </row>
-    <row r="37" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y36" s="43" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
         <v>37</v>
       </c>
@@ -3461,7 +3479,7 @@
       <c r="W37" s="31"/>
       <c r="X37" s="75"/>
     </row>
-    <row r="38" spans="1:26" s="32" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:26" s="32" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>272</v>
       </c>
@@ -3487,7 +3505,7 @@
       </c>
       <c r="Z38" s="50"/>
     </row>
-    <row r="39" spans="1:26" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:26" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
@@ -3522,7 +3540,7 @@
       <c r="W39" s="31"/>
       <c r="X39" s="75"/>
     </row>
-    <row r="40" spans="1:26" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:26" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>41</v>
       </c>
@@ -3563,7 +3581,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="41" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>43</v>
       </c>
@@ -3598,7 +3616,7 @@
       <c r="W41" s="31"/>
       <c r="X41" s="75"/>
     </row>
-    <row r="42" spans="1:26" s="25" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:26" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
         <v>254</v>
       </c>
@@ -3636,7 +3654,7 @@
       <c r="W42" s="59"/>
       <c r="X42" s="75"/>
     </row>
-    <row r="43" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>173</v>
       </c>
@@ -3681,7 +3699,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="44" spans="1:26" s="4" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:26" s="4" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A44" s="32" t="s">
         <v>45</v>
       </c>
@@ -3718,7 +3736,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="45" spans="1:26" s="4" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:26" s="4" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="44" t="s">
         <v>47</v>
       </c>
@@ -3752,7 +3770,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="46" spans="1:26" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:26" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="77" t="s">
         <v>50</v>
       </c>
@@ -3792,7 +3810,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="47" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="77"/>
       <c r="B47" s="77"/>
       <c r="C47" s="77"/>
@@ -3814,7 +3832,7 @@
       <c r="X47" s="75"/>
       <c r="Y47" s="76"/>
     </row>
-    <row r="48" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>175</v>
       </c>
@@ -3846,7 +3864,7 @@
       <c r="W48" s="31"/>
       <c r="X48" s="75"/>
     </row>
-    <row r="49" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>52</v>
       </c>
@@ -3880,7 +3898,7 @@
       <c r="W49" s="31"/>
       <c r="X49" s="75"/>
     </row>
-    <row r="50" spans="1:26" s="1" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:26" s="1" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
         <v>54</v>
       </c>
@@ -3920,7 +3938,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="51" spans="1:26" s="1" customFormat="1" ht="160.30000000000001" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:26" s="1" customFormat="1" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>213</v>
       </c>
@@ -3992,7 +4010,7 @@
       </c>
       <c r="Z51"/>
     </row>
-    <row r="52" spans="1:26" s="4" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:26" s="4" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="32" t="s">
         <v>178</v>
       </c>
@@ -4018,7 +4036,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="53" spans="1:26" s="4" customFormat="1" ht="86.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:26" s="4" customFormat="1" ht="86.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="32" t="s">
         <v>180</v>
       </c>
@@ -4057,7 +4075,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="54" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
         <v>57</v>
       </c>
@@ -4090,7 +4108,7 @@
       <c r="X54" s="75"/>
       <c r="Y54" s="43"/>
     </row>
-    <row r="55" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
         <v>59</v>
       </c>
@@ -4128,7 +4146,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="56" spans="1:26" s="4" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:26" s="4" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
         <v>61</v>
       </c>
@@ -4160,7 +4178,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="57" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="s">
         <v>183</v>
       </c>
@@ -4195,7 +4213,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="58" spans="1:26" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:26" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A58" s="65" t="s">
         <v>278</v>
       </c>
@@ -4232,7 +4250,7 @@
       </c>
       <c r="Z58" s="50"/>
     </row>
-    <row r="59" spans="1:26" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:26" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="s">
         <v>280</v>
       </c>
@@ -4257,7 +4275,7 @@
       </c>
       <c r="Z59" s="50"/>
     </row>
-    <row r="60" spans="1:26" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:26" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="s">
         <v>185</v>
       </c>
@@ -4280,7 +4298,7 @@
       <c r="Y60" s="43"/>
       <c r="Z60" s="50"/>
     </row>
-    <row r="61" spans="1:26" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:26" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A61" s="4" t="s">
         <v>283</v>
       </c>
@@ -4315,7 +4333,7 @@
       </c>
       <c r="Z61" s="50"/>
     </row>
-    <row r="62" spans="1:26" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:26" ht="29" x14ac:dyDescent="0.35">
       <c r="A62" s="11" t="s">
         <v>233</v>
       </c>
@@ -4357,7 +4375,7 @@
       </c>
       <c r="Z62" s="50"/>
     </row>
-    <row r="63" spans="1:26" s="4" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:26" s="4" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A63" s="4" t="s">
         <v>187</v>
       </c>
@@ -4383,7 +4401,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="64" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="4" t="s">
         <v>63</v>
       </c>
@@ -4419,7 +4437,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="65" spans="1:26" s="37" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:26" s="37" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="s">
         <v>295</v>
       </c>
@@ -4450,7 +4468,7 @@
       </c>
       <c r="Z65" s="61"/>
     </row>
-    <row r="66" spans="1:26" s="4" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:26" s="4" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A66" s="4" t="s">
         <v>65</v>
       </c>
@@ -4476,7 +4494,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="67" spans="1:26" s="4" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:26" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A67" s="4" t="s">
         <v>297</v>
       </c>
@@ -4497,7 +4515,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="68" spans="1:26" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:26" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A68" s="65" t="s">
         <v>252</v>
       </c>
@@ -4521,7 +4539,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="69" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>68</v>
       </c>
@@ -4555,7 +4573,7 @@
       <c r="W69" s="31"/>
       <c r="X69" s="75"/>
     </row>
-    <row r="70" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>70</v>
       </c>
@@ -4590,7 +4608,7 @@
       <c r="W70" s="31"/>
       <c r="X70" s="45"/>
     </row>
-    <row r="71" spans="1:26" s="19" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:26" s="19" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A71" s="19" t="s">
         <v>244</v>
       </c>
@@ -4629,7 +4647,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="72" spans="1:26" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:26" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>189</v>
       </c>
@@ -4666,7 +4684,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="73" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>72</v>
       </c>
@@ -4734,7 +4752,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="74" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A74" s="35" t="s">
         <v>192</v>
       </c>
@@ -4766,7 +4784,7 @@
       <c r="W74" s="59"/>
       <c r="X74" s="75"/>
     </row>
-    <row r="75" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A75" s="32" t="s">
         <v>74</v>
       </c>
@@ -4801,7 +4819,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="76" spans="1:26" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:26" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A76" s="32" t="s">
         <v>419</v>
       </c>
@@ -4832,7 +4850,7 @@
       <c r="Y76" s="42"/>
       <c r="Z76" s="73"/>
     </row>
-    <row r="77" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>211</v>
       </c>
@@ -4866,7 +4884,7 @@
       <c r="W77" s="31"/>
       <c r="X77" s="75"/>
     </row>
-    <row r="78" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>76</v>
       </c>
@@ -4901,7 +4919,7 @@
       <c r="W78" s="31"/>
       <c r="X78" s="32"/>
     </row>
-    <row r="79" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>78</v>
       </c>
@@ -4969,7 +4987,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="80" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>80</v>
       </c>
@@ -5004,7 +5022,7 @@
       <c r="W80" s="31"/>
       <c r="X80" s="45"/>
     </row>
-    <row r="81" spans="1:26" s="4" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:26" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A81" s="4" t="s">
         <v>83</v>
       </c>
@@ -5039,7 +5057,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="82" spans="1:26" s="4" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:26" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A82" s="4" t="s">
         <v>301</v>
       </c>
@@ -5061,7 +5079,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="83" spans="1:26" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:26" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>193</v>
       </c>
@@ -5099,7 +5117,7 @@
       </c>
       <c r="Z83" s="4"/>
     </row>
-    <row r="84" spans="1:26" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:26" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A84" s="4" t="s">
         <v>303</v>
       </c>
@@ -5122,7 +5140,7 @@
       </c>
       <c r="Z84" s="4"/>
     </row>
-    <row r="85" spans="1:26" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:26" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A85" s="4" t="s">
         <v>306</v>
       </c>
@@ -5145,7 +5163,7 @@
       </c>
       <c r="Z85" s="4"/>
     </row>
-    <row r="86" spans="1:26" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:26" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A86" s="4" t="s">
         <v>309</v>
       </c>
@@ -5168,7 +5186,7 @@
       </c>
       <c r="Z86" s="4"/>
     </row>
-    <row r="87" spans="1:26" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:26" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A87" s="4" t="s">
         <v>312</v>
       </c>
@@ -5191,7 +5209,7 @@
       </c>
       <c r="Z87" s="4"/>
     </row>
-    <row r="88" spans="1:26" s="4" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:26" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A88" s="4" t="s">
         <v>196</v>
       </c>
@@ -5217,7 +5235,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="89" spans="1:26" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:26" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>85</v>
       </c>
@@ -5291,7 +5309,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="90" spans="1:26" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:26" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>87</v>
       </c>
@@ -5332,7 +5350,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="91" spans="1:26" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:26" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A91" s="4" t="s">
         <v>91</v>
       </c>
@@ -5364,7 +5382,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="92" spans="1:26" s="4" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:26" s="4" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="4" t="s">
         <v>147</v>
       </c>
@@ -5390,7 +5408,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="93" spans="1:26" s="4" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:26" s="4" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="32" t="s">
         <v>424</v>
       </c>
@@ -5423,7 +5441,7 @@
       </c>
       <c r="Y93" s="58"/>
     </row>
-    <row r="94" spans="1:26" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:26" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
         <v>95</v>
       </c>
@@ -5458,7 +5476,7 @@
       <c r="W94" s="31"/>
       <c r="X94" s="45"/>
     </row>
-    <row r="95" spans="1:26" s="38" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:26" s="38" customFormat="1" ht="116" x14ac:dyDescent="0.35">
       <c r="A95" s="60" t="s">
         <v>314</v>
       </c>
@@ -5490,7 +5508,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="96" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:26" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A96" s="60" t="s">
         <v>218</v>
       </c>
@@ -5527,7 +5545,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="97" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
         <v>149</v>
       </c>
@@ -5567,7 +5585,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="98" spans="1:26" s="26" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:26" s="26" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A98" s="26" t="s">
         <v>98</v>
       </c>
@@ -5603,7 +5621,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="99" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A99" s="4" t="s">
         <v>198</v>
       </c>
@@ -5640,7 +5658,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="100" spans="1:26" s="9" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:26" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A100" s="4" t="s">
         <v>240</v>
       </c>
@@ -5675,7 +5693,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="101" spans="1:26" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:26" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A101" s="4" t="s">
         <v>214</v>
       </c>
@@ -5715,7 +5733,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="102" spans="1:26" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:26" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
         <v>100</v>
       </c>
@@ -5749,7 +5767,7 @@
       <c r="W102" s="31"/>
       <c r="X102" s="75"/>
     </row>
-    <row r="103" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A103" s="5" t="s">
         <v>274</v>
       </c>
@@ -5773,7 +5791,7 @@
       <c r="M103" s="22"/>
       <c r="S103" s="22"/>
     </row>
-    <row r="104" spans="1:26" s="1" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:26" s="1" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
         <v>102</v>
       </c>
@@ -5814,7 +5832,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="105" spans="1:26" s="38" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:26" s="38" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A105" s="61" t="s">
         <v>318</v>
       </c>
@@ -5858,7 +5876,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="106" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
         <v>104</v>
       </c>
@@ -5892,7 +5910,7 @@
       <c r="W106" s="31"/>
       <c r="X106" s="75"/>
     </row>
-    <row r="107" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
         <v>201</v>
       </c>
@@ -5926,7 +5944,7 @@
       <c r="W107" s="31"/>
       <c r="X107" s="75"/>
     </row>
-    <row r="108" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
         <v>106</v>
       </c>
@@ -5960,7 +5978,7 @@
       <c r="W108" s="31"/>
       <c r="X108" s="75"/>
     </row>
-    <row r="109" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
         <v>110</v>
       </c>
@@ -6028,7 +6046,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="110" spans="1:26" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:26" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A110" s="4" t="s">
         <v>112</v>
       </c>
@@ -6063,7 +6081,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="111" spans="1:26" s="4" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:26" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A111" s="4" t="s">
         <v>114</v>
       </c>
@@ -6093,7 +6111,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="112" spans="1:26" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:26" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>116</v>
       </c>
@@ -6126,7 +6144,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="113" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
         <v>118</v>
       </c>
@@ -6188,7 +6206,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A114" s="60" t="s">
         <v>120</v>
       </c>
@@ -6250,7 +6268,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A115" s="60" t="s">
         <v>121</v>
       </c>
@@ -6301,7 +6319,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A116" s="4" t="s">
         <v>151</v>
       </c>
@@ -6337,7 +6355,7 @@
       <c r="W116" s="31"/>
       <c r="X116" s="75"/>
     </row>
-    <row r="117" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A117" s="5" t="s">
         <v>276</v>
       </c>
@@ -6373,7 +6391,7 @@
       <c r="W117"/>
       <c r="X117"/>
     </row>
-    <row r="118" spans="1:26" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:26" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A118" s="44" t="s">
         <v>123</v>
       </c>
@@ -6434,7 +6452,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="119" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A119" s="60" t="s">
         <v>126</v>
       </c>
@@ -6496,7 +6514,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A120" s="60" t="s">
         <v>232</v>
       </c>
@@ -6558,7 +6576,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="121" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A121" s="60" t="s">
         <v>129</v>
       </c>
@@ -6593,7 +6611,7 @@
       <c r="W121" s="31"/>
       <c r="X121" s="45"/>
     </row>
-    <row r="122" spans="1:26" s="71" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:26" s="71" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A122" s="72" t="s">
         <v>417</v>
       </c>
@@ -6659,7 +6677,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="123" spans="1:26" s="20" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:26" s="20" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A123" s="60" t="s">
         <v>247</v>
       </c>
@@ -6701,7 +6719,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="124" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A124" s="60" t="s">
         <v>131</v>
       </c>
@@ -6745,7 +6763,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="125" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A125" s="41"/>
       <c r="B125" s="41"/>
       <c r="C125" s="41"/>
@@ -6757,7 +6775,7 @@
       <c r="N125" s="45"/>
       <c r="S125" s="22"/>
     </row>
-    <row r="126" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A126" s="41"/>
       <c r="B126" s="41"/>
       <c r="C126" s="41"/>
@@ -6768,7 +6786,7 @@
       <c r="H126" s="39"/>
       <c r="S126" s="22"/>
     </row>
-    <row r="127" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A127" s="41"/>
       <c r="B127" s="41"/>
       <c r="C127" s="41"/>
@@ -6779,7 +6797,7 @@
       <c r="H127" s="39"/>
       <c r="S127" s="22"/>
     </row>
-    <row r="128" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A128" s="41"/>
       <c r="B128" s="41"/>
       <c r="C128" s="41"/>
@@ -6790,7 +6808,7 @@
       <c r="H128" s="39"/>
       <c r="S128" s="22"/>
     </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A129" s="41"/>
       <c r="B129" s="41"/>
       <c r="C129" s="41"/>
@@ -6801,7 +6819,7 @@
       <c r="H129" s="39"/>
       <c r="S129" s="22"/>
     </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A130" s="41"/>
       <c r="B130" s="41"/>
       <c r="C130" s="41"/>
@@ -6812,7 +6830,7 @@
       <c r="H130" s="39"/>
       <c r="S130" s="22"/>
     </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A131" s="41"/>
       <c r="B131" s="41"/>
       <c r="C131" s="41"/>
@@ -6823,7 +6841,7 @@
       <c r="H131" s="39"/>
       <c r="S131" s="22"/>
     </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="132" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A132" s="41"/>
       <c r="B132" s="41"/>
       <c r="C132" s="41"/>
@@ -6834,7 +6852,7 @@
       <c r="H132" s="39"/>
       <c r="S132" s="22"/>
     </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A133" s="41"/>
       <c r="B133" s="41"/>
       <c r="C133" s="41"/>
@@ -6845,7 +6863,7 @@
       <c r="H133" s="39"/>
       <c r="S133" s="22"/>
     </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A134" s="41"/>
       <c r="B134" s="41"/>
       <c r="C134" s="41"/>
@@ -6855,7 +6873,7 @@
       <c r="G134" s="48"/>
       <c r="S134" s="22"/>
     </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A135" s="41"/>
       <c r="B135" s="41"/>
       <c r="C135" s="41"/>
@@ -6865,7 +6883,7 @@
       <c r="G135" s="48"/>
       <c r="S135" s="22"/>
     </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A136" s="41"/>
       <c r="B136" s="41"/>
       <c r="C136" s="41"/>
@@ -6875,7 +6893,7 @@
       <c r="G136" s="48"/>
       <c r="S136" s="22"/>
     </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A137" s="41"/>
       <c r="B137" s="41"/>
       <c r="C137" s="41"/>
@@ -6885,7 +6903,7 @@
       <c r="G137" s="48"/>
       <c r="S137" s="22"/>
     </row>
-    <row r="138" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A138" s="41"/>
       <c r="B138" s="41"/>
       <c r="C138" s="41"/>
@@ -6895,7 +6913,7 @@
       <c r="G138" s="48"/>
       <c r="S138" s="22"/>
     </row>
-    <row r="139" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A139" s="41"/>
       <c r="B139" s="41"/>
       <c r="C139" s="41"/>
@@ -6905,7 +6923,7 @@
       <c r="G139" s="48"/>
       <c r="S139" s="22"/>
     </row>
-    <row r="140" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A140" s="41"/>
       <c r="B140" s="41"/>
       <c r="C140" s="41"/>
@@ -6915,7 +6933,7 @@
       <c r="G140" s="48"/>
       <c r="S140" s="22"/>
     </row>
-    <row r="141" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A141" s="41"/>
       <c r="B141" s="41"/>
       <c r="C141" s="41"/>
@@ -6925,7 +6943,7 @@
       <c r="G141" s="48"/>
       <c r="S141" s="22"/>
     </row>
-    <row r="142" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A142" s="41"/>
       <c r="B142" s="41"/>
       <c r="C142" s="41"/>
@@ -6935,7 +6953,7 @@
       <c r="G142" s="48"/>
       <c r="S142" s="22"/>
     </row>
-    <row r="143" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A143" s="41"/>
       <c r="B143" s="41"/>
       <c r="C143" s="41"/>
@@ -6945,7 +6963,7 @@
       <c r="G143" s="48"/>
       <c r="S143" s="22"/>
     </row>
-    <row r="144" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A144" s="41"/>
       <c r="B144" s="41"/>
       <c r="C144" s="41"/>
@@ -6955,7 +6973,7 @@
       <c r="G144" s="48"/>
       <c r="S144" s="22"/>
     </row>
-    <row r="145" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A145" s="41"/>
       <c r="B145" s="41"/>
       <c r="C145" s="41"/>
@@ -6965,7 +6983,7 @@
       <c r="G145" s="48"/>
       <c r="S145" s="22"/>
     </row>
-    <row r="146" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A146" s="41"/>
       <c r="B146" s="41"/>
       <c r="C146" s="41"/>
@@ -6975,7 +6993,7 @@
       <c r="G146" s="48"/>
       <c r="S146" s="22"/>
     </row>
-    <row r="147" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A147" s="41"/>
       <c r="B147" s="41"/>
       <c r="C147" s="41"/>
@@ -6985,7 +7003,7 @@
       <c r="G147" s="48"/>
       <c r="S147" s="22"/>
     </row>
-    <row r="148" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A148" s="41"/>
       <c r="B148" s="41"/>
       <c r="C148" s="41"/>
@@ -6995,7 +7013,7 @@
       <c r="G148" s="48"/>
       <c r="S148" s="22"/>
     </row>
-    <row r="149" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A149" s="41"/>
       <c r="B149" s="41"/>
       <c r="C149" s="41"/>
@@ -7005,7 +7023,7 @@
       <c r="G149" s="48"/>
       <c r="S149" s="22"/>
     </row>
-    <row r="150" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A150" s="41"/>
       <c r="B150" s="41"/>
       <c r="C150" s="41"/>
@@ -7015,7 +7033,7 @@
       <c r="G150" s="48"/>
       <c r="S150" s="22"/>
     </row>
-    <row r="151" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A151" s="41"/>
       <c r="B151" s="41"/>
       <c r="C151" s="41"/>
@@ -7025,7 +7043,7 @@
       <c r="G151" s="48"/>
       <c r="S151" s="22"/>
     </row>
-    <row r="152" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A152" s="41"/>
       <c r="B152" s="41"/>
       <c r="C152" s="41"/>
@@ -7035,7 +7053,7 @@
       <c r="G152" s="48"/>
       <c r="S152" s="22"/>
     </row>
-    <row r="153" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A153" s="41"/>
       <c r="B153" s="41"/>
       <c r="C153" s="41"/>
@@ -7045,7 +7063,7 @@
       <c r="G153" s="48"/>
       <c r="S153" s="22"/>
     </row>
-    <row r="154" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="154" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A154" s="41"/>
       <c r="B154" s="41"/>
       <c r="C154" s="41"/>
@@ -7055,7 +7073,7 @@
       <c r="G154" s="48"/>
       <c r="S154" s="22"/>
     </row>
-    <row r="155" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="155" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A155" s="41"/>
       <c r="B155" s="41"/>
       <c r="C155" s="41"/>
@@ -7066,22 +7084,22 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="Y46:Y47"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
     <mergeCell ref="Y7:Y8"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="Y46:Y47"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="H20" r:id="rId1" display="standaarden.ondersteuning@vng.nl"/>
-    <hyperlink ref="F20" r:id="rId2"/>
-    <hyperlink ref="F45" r:id="rId3"/>
+    <hyperlink ref="H20" r:id="rId1" display="standaarden.ondersteuning@vng.nl" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F20" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F45" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="37" fitToHeight="0" orientation="landscape" r:id="rId4"/>
@@ -7089,25 +7107,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.69140625" customWidth="1"/>
-    <col min="2" max="2" width="52.23046875" customWidth="1"/>
+    <col min="1" max="1" width="18.7265625" customWidth="1"/>
+    <col min="2" max="2" width="52.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>229</v>
       </c>
@@ -7115,7 +7133,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>230</v>
       </c>
@@ -7123,8 +7141,8 @@
         <v>228</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="6" spans="1:2" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="6" spans="1:2" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="3" t="s">
         <v>208</v>
       </c>
@@ -7132,7 +7150,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:2" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="3" t="s">
         <v>209</v>
       </c>
@@ -7140,7 +7158,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:2" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="3" t="s">
         <v>210</v>
       </c>
@@ -7148,7 +7166,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.4"/>
+    <row r="9" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
KING: MUG als metamodel vervangen voor MBG
Het MUG is niet expliciet beschreven door VNGR als metamodel, maar
opgenomen in MBG. Op verzoek is de naam MUG in de configuraties
vervangen door MBG.
Deze aanpassing heeft geen inhoudelijke implicaties. Heft betreft alleen
naamgeving.

Refactoring.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/KING/props/KING.xlsx
+++ b/src/main/resources/input/KING/props/KING.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\KING\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6212211-7FAF-478E-9E6B-0C80F03C7416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A71B42-69F2-4EB4-823F-302ED1BB43CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="20057" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1369,10 +1369,10 @@
     <t>1.1</t>
   </si>
   <si>
-    <t>MUG</t>
-  </si>
-  <si>
     <t>1.0</t>
+  </si>
+  <si>
+    <t>MBG</t>
   </si>
 </sst>
 </file>
@@ -1572,7 +1572,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1683,9 +1683,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1980,11 +1977,11 @@
   <dimension ref="A1:Z159"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="G63" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E64" sqref="E64"/>
       <selection pane="topRight" activeCell="E64" sqref="E64"/>
       <selection pane="bottomLeft" activeCell="E64" sqref="E64"/>
-      <selection pane="bottomRight" activeCell="U74" sqref="U74:X76"/>
+      <selection pane="bottomRight" activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4092,52 +4089,52 @@
       </c>
       <c r="F74" s="26"/>
       <c r="G74" s="12"/>
-      <c r="H74" s="44" t="s">
+      <c r="H74" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="I74" s="44" t="s">
+      <c r="I74" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="J74" s="44" t="s">
+      <c r="J74" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="K74" s="44" t="s">
+      <c r="K74" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="L74" s="44" t="s">
+      <c r="L74" s="1" t="s">
         <v>430</v>
       </c>
       <c r="M74" s="12"/>
       <c r="N74" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="O74" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="P74" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="Q74" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="R74" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="S74" s="12"/>
       <c r="T74" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="U74" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="V74" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="W74" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="X74" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="75" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -4158,52 +4155,52 @@
       </c>
       <c r="F75" s="26"/>
       <c r="G75" s="12"/>
-      <c r="H75" s="44" t="s">
+      <c r="H75" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="I75" s="44" t="s">
+      <c r="I75" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="J75" s="44" t="s">
+      <c r="J75" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="K75" s="44" t="s">
+      <c r="K75" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="L75" s="44" t="s">
+      <c r="L75" s="1" t="s">
         <v>437</v>
       </c>
       <c r="M75" s="12"/>
       <c r="N75" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="O75" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="P75" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="Q75" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="R75" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="S75" s="12"/>
       <c r="T75" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="U75" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="V75" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="W75" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="X75" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="76" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -6209,16 +6206,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="Y46:Y47"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
     <mergeCell ref="Y7:Y8"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="Y46:Y47"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <hyperlinks>

</xml_diff>